<commit_message>
hardware: outputs: board_bom: Manually fixing PC104 component quantity and adding missing partnumbers on pin headers close #186
</commit_message>
<xml_diff>
--- a/hardware/outputs/board_bom/board_bom.xlsx
+++ b/hardware/outputs/board_bom/board_bom.xlsx
@@ -1,11 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23328"/>
   <workbookPr/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{E6B24226-3C1E-46E8-9D11-07EDC9479674}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Yan Azeredo\Desktop\SpaceLab\obdh2\hardware\outputs\board_bom\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{24D879F6-8532-4A71-BEB0-7E1C86E42973}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1500" yWindow="0" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Plan1" sheetId="1" r:id="rId1"/>
@@ -32,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="215" uniqueCount="161">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="215" uniqueCount="163">
   <si>
     <t>Source Data From:</t>
   </si>
@@ -157,9 +162,6 @@
     <t>FSI-110-03-G-D-AD</t>
   </si>
   <si>
-    <t/>
-  </si>
-  <si>
     <t>MAX9934TAUA+</t>
   </si>
   <si>
@@ -515,6 +517,15 @@
   </si>
   <si>
     <t>Fitted</t>
+  </si>
+  <si>
+    <t>M20-9990445</t>
+  </si>
+  <si>
+    <t>M20-9980745</t>
+  </si>
+  <si>
+    <t>M20-9990645</t>
   </si>
 </sst>
 </file>
@@ -754,11 +765,11 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="9" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="5" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -766,23 +777,23 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="9" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="5" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1392,7 +1403,7 @@
   <dimension ref="A1:J69"/>
   <sheetViews>
     <sheetView tabSelected="1" view="pageBreakPreview" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+      <selection activeCell="C40" sqref="C40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1412,14 +1423,14 @@
     <row r="1" spans="1:10" ht="28.5" x14ac:dyDescent="0.25">
       <c r="A1" s="1"/>
       <c r="B1" s="7"/>
-      <c r="C1" s="26" t="s">
+      <c r="C1" s="25" t="s">
         <v>6</v>
       </c>
-      <c r="D1" s="26"/>
-      <c r="E1" s="26"/>
-      <c r="F1" s="26"/>
-      <c r="G1" s="26"/>
-      <c r="H1" s="26"/>
+      <c r="D1" s="25"/>
+      <c r="E1" s="25"/>
+      <c r="F1" s="25"/>
+      <c r="G1" s="25"/>
+      <c r="H1" s="25"/>
       <c r="I1" s="2"/>
       <c r="J1" s="2"/>
     </row>
@@ -1429,7 +1440,7 @@
       <c r="C2" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="D2" s="28" t="s">
+      <c r="D2" s="26" t="s">
         <v>8</v>
       </c>
       <c r="E2" s="27"/>
@@ -1445,7 +1456,7 @@
       <c r="C3" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="D3" s="28" t="s">
+      <c r="D3" s="26" t="s">
         <v>8</v>
       </c>
       <c r="E3" s="27"/>
@@ -1461,7 +1472,7 @@
       <c r="C4" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="D4" s="28" t="s">
+      <c r="D4" s="26" t="s">
         <v>9</v>
       </c>
       <c r="E4" s="27"/>
@@ -1477,7 +1488,7 @@
       <c r="C5" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="D5" s="28" t="s">
+      <c r="D5" s="26" t="s">
         <v>10</v>
       </c>
       <c r="E5" s="27"/>
@@ -1490,11 +1501,11 @@
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" s="4"/>
       <c r="B6" s="7"/>
-      <c r="C6" s="25"/>
-      <c r="D6" s="25"/>
-      <c r="E6" s="25"/>
-      <c r="F6" s="25"/>
-      <c r="G6" s="25"/>
+      <c r="C6" s="30"/>
+      <c r="D6" s="30"/>
+      <c r="E6" s="30"/>
+      <c r="F6" s="30"/>
+      <c r="G6" s="30"/>
       <c r="H6" s="20"/>
       <c r="I6" s="2"/>
       <c r="J6" s="2"/>
@@ -1505,10 +1516,10 @@
       <c r="C7" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="D7" s="29" t="s">
+      <c r="D7" s="21" t="s">
         <v>11</v>
       </c>
-      <c r="E7" s="29" t="s">
+      <c r="E7" s="21" t="s">
         <v>12</v>
       </c>
       <c r="F7" s="9"/>
@@ -1525,11 +1536,11 @@
       </c>
       <c r="D8" s="11">
         <f ca="1">TODAY()</f>
-        <v>44069</v>
+        <v>44156</v>
       </c>
       <c r="E8" s="12">
         <f ca="1">NOW()</f>
-        <v>44069.855479513892</v>
+        <v>44156.906615624997</v>
       </c>
       <c r="F8" s="9"/>
       <c r="G8" s="9"/>
@@ -1550,27 +1561,27 @@
       <c r="J9" s="2"/>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A10" s="21" t="s">
+      <c r="A10" s="28" t="s">
         <v>5</v>
       </c>
-      <c r="B10" s="22"/>
+      <c r="B10" s="29"/>
       <c r="C10" s="16" t="s">
         <v>13</v>
       </c>
       <c r="D10" s="16" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="E10" s="16" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="F10" s="16" t="s">
+        <v>118</v>
+      </c>
+      <c r="G10" s="16" t="s">
         <v>119</v>
       </c>
-      <c r="G10" s="16" t="s">
-        <v>120</v>
-      </c>
       <c r="H10" s="16" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="I10" s="17"/>
     </row>
@@ -1580,48 +1591,48 @@
         <v>1</v>
       </c>
       <c r="B11" s="24"/>
-      <c r="C11" s="30" t="s">
+      <c r="C11" s="22" t="s">
         <v>14</v>
       </c>
-      <c r="D11" s="30" t="s">
-        <v>51</v>
-      </c>
-      <c r="E11" s="30" t="s">
-        <v>84</v>
+      <c r="D11" s="22" t="s">
+        <v>50</v>
+      </c>
+      <c r="E11" s="22" t="s">
+        <v>83</v>
       </c>
       <c r="F11" s="18">
         <v>22</v>
       </c>
-      <c r="G11" s="30" t="s">
-        <v>121</v>
-      </c>
-      <c r="H11" s="30" t="s">
-        <v>160</v>
+      <c r="G11" s="22" t="s">
+        <v>120</v>
+      </c>
+      <c r="H11" s="22" t="s">
+        <v>159</v>
       </c>
     </row>
     <row r="12" spans="1:10" ht="76.5" x14ac:dyDescent="0.25">
       <c r="A12" s="23">
-        <f t="shared" ref="A12:A49" si="0">ROW(A12) - ROW($A$10)</f>
+        <f t="shared" ref="A12:A48" si="0">ROW(A12) - ROW($A$10)</f>
         <v>2</v>
       </c>
       <c r="B12" s="24"/>
-      <c r="C12" s="30" t="s">
+      <c r="C12" s="22" t="s">
         <v>15</v>
       </c>
-      <c r="D12" s="30" t="s">
-        <v>52</v>
-      </c>
-      <c r="E12" s="30" t="s">
-        <v>85</v>
+      <c r="D12" s="22" t="s">
+        <v>51</v>
+      </c>
+      <c r="E12" s="22" t="s">
+        <v>84</v>
       </c>
       <c r="F12" s="18">
         <v>17</v>
       </c>
-      <c r="G12" s="30" t="s">
-        <v>122</v>
-      </c>
-      <c r="H12" s="30" t="s">
-        <v>160</v>
+      <c r="G12" s="22" t="s">
+        <v>121</v>
+      </c>
+      <c r="H12" s="22" t="s">
+        <v>159</v>
       </c>
     </row>
     <row r="13" spans="1:10" ht="38.25" x14ac:dyDescent="0.25">
@@ -1630,23 +1641,23 @@
         <v>3</v>
       </c>
       <c r="B13" s="24"/>
-      <c r="C13" s="30" t="s">
+      <c r="C13" s="22" t="s">
         <v>16</v>
       </c>
-      <c r="D13" s="30" t="s">
-        <v>53</v>
-      </c>
-      <c r="E13" s="30" t="s">
-        <v>86</v>
+      <c r="D13" s="22" t="s">
+        <v>52</v>
+      </c>
+      <c r="E13" s="22" t="s">
+        <v>85</v>
       </c>
       <c r="F13" s="18">
         <v>14</v>
       </c>
-      <c r="G13" s="30" t="s">
-        <v>123</v>
-      </c>
-      <c r="H13" s="30" t="s">
-        <v>160</v>
+      <c r="G13" s="22" t="s">
+        <v>122</v>
+      </c>
+      <c r="H13" s="22" t="s">
+        <v>159</v>
       </c>
     </row>
     <row r="14" spans="1:10" ht="25.5" x14ac:dyDescent="0.25">
@@ -1655,23 +1666,23 @@
         <v>4</v>
       </c>
       <c r="B14" s="24"/>
-      <c r="C14" s="30" t="s">
+      <c r="C14" s="22" t="s">
         <v>17</v>
       </c>
-      <c r="D14" s="30" t="s">
-        <v>54</v>
-      </c>
-      <c r="E14" s="30" t="s">
-        <v>87</v>
+      <c r="D14" s="22" t="s">
+        <v>53</v>
+      </c>
+      <c r="E14" s="22" t="s">
+        <v>86</v>
       </c>
       <c r="F14" s="18">
         <v>8</v>
       </c>
-      <c r="G14" s="30" t="s">
-        <v>124</v>
-      </c>
-      <c r="H14" s="30" t="s">
-        <v>160</v>
+      <c r="G14" s="22" t="s">
+        <v>123</v>
+      </c>
+      <c r="H14" s="22" t="s">
+        <v>159</v>
       </c>
     </row>
     <row r="15" spans="1:10" ht="25.5" x14ac:dyDescent="0.25">
@@ -1680,23 +1691,23 @@
         <v>5</v>
       </c>
       <c r="B15" s="24"/>
-      <c r="C15" s="30" t="s">
+      <c r="C15" s="22" t="s">
         <v>18</v>
       </c>
-      <c r="D15" s="30" t="s">
-        <v>55</v>
-      </c>
-      <c r="E15" s="30" t="s">
-        <v>88</v>
+      <c r="D15" s="22" t="s">
+        <v>54</v>
+      </c>
+      <c r="E15" s="22" t="s">
+        <v>87</v>
       </c>
       <c r="F15" s="18">
         <v>7</v>
       </c>
-      <c r="G15" s="30" t="s">
-        <v>125</v>
-      </c>
-      <c r="H15" s="30" t="s">
-        <v>160</v>
+      <c r="G15" s="22" t="s">
+        <v>124</v>
+      </c>
+      <c r="H15" s="22" t="s">
+        <v>159</v>
       </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.25">
@@ -1705,23 +1716,23 @@
         <v>6</v>
       </c>
       <c r="B16" s="24"/>
-      <c r="C16" s="30" t="s">
+      <c r="C16" s="22" t="s">
         <v>19</v>
       </c>
-      <c r="D16" s="30" t="s">
-        <v>56</v>
-      </c>
-      <c r="E16" s="30" t="s">
-        <v>89</v>
+      <c r="D16" s="22" t="s">
+        <v>55</v>
+      </c>
+      <c r="E16" s="22" t="s">
+        <v>88</v>
       </c>
       <c r="F16" s="18">
         <v>6</v>
       </c>
-      <c r="G16" s="30" t="s">
-        <v>126</v>
-      </c>
-      <c r="H16" s="30" t="s">
-        <v>160</v>
+      <c r="G16" s="22" t="s">
+        <v>125</v>
+      </c>
+      <c r="H16" s="22" t="s">
+        <v>159</v>
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">
@@ -1730,23 +1741,23 @@
         <v>7</v>
       </c>
       <c r="B17" s="24"/>
-      <c r="C17" s="30" t="s">
+      <c r="C17" s="22" t="s">
         <v>20</v>
       </c>
-      <c r="D17" s="30" t="s">
-        <v>57</v>
-      </c>
-      <c r="E17" s="30" t="s">
-        <v>90</v>
+      <c r="D17" s="22" t="s">
+        <v>56</v>
+      </c>
+      <c r="E17" s="22" t="s">
+        <v>89</v>
       </c>
       <c r="F17" s="18">
         <v>6</v>
       </c>
-      <c r="G17" s="30" t="s">
-        <v>127</v>
-      </c>
-      <c r="H17" s="30" t="s">
-        <v>160</v>
+      <c r="G17" s="22" t="s">
+        <v>126</v>
+      </c>
+      <c r="H17" s="22" t="s">
+        <v>159</v>
       </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.25">
@@ -1755,23 +1766,23 @@
         <v>8</v>
       </c>
       <c r="B18" s="24"/>
-      <c r="C18" s="30" t="s">
+      <c r="C18" s="22" t="s">
         <v>21</v>
       </c>
-      <c r="D18" s="30" t="s">
-        <v>58</v>
-      </c>
-      <c r="E18" s="30" t="s">
-        <v>91</v>
+      <c r="D18" s="22" t="s">
+        <v>57</v>
+      </c>
+      <c r="E18" s="22" t="s">
+        <v>90</v>
       </c>
       <c r="F18" s="18">
         <v>4</v>
       </c>
-      <c r="G18" s="30" t="s">
-        <v>128</v>
-      </c>
-      <c r="H18" s="30" t="s">
-        <v>160</v>
+      <c r="G18" s="22" t="s">
+        <v>127</v>
+      </c>
+      <c r="H18" s="22" t="s">
+        <v>159</v>
       </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.25">
@@ -1780,23 +1791,23 @@
         <v>9</v>
       </c>
       <c r="B19" s="24"/>
-      <c r="C19" s="30" t="s">
+      <c r="C19" s="22" t="s">
         <v>22</v>
       </c>
-      <c r="D19" s="30" t="s">
-        <v>59</v>
-      </c>
-      <c r="E19" s="30" t="s">
-        <v>92</v>
+      <c r="D19" s="22" t="s">
+        <v>58</v>
+      </c>
+      <c r="E19" s="22" t="s">
+        <v>91</v>
       </c>
       <c r="F19" s="18">
         <v>4</v>
       </c>
-      <c r="G19" s="30" t="s">
-        <v>129</v>
-      </c>
-      <c r="H19" s="30" t="s">
-        <v>160</v>
+      <c r="G19" s="22" t="s">
+        <v>128</v>
+      </c>
+      <c r="H19" s="22" t="s">
+        <v>159</v>
       </c>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.25">
@@ -1805,23 +1816,23 @@
         <v>10</v>
       </c>
       <c r="B20" s="24"/>
-      <c r="C20" s="30" t="s">
+      <c r="C20" s="22" t="s">
         <v>23</v>
       </c>
-      <c r="D20" s="30" t="s">
+      <c r="D20" s="22" t="s">
         <v>23</v>
       </c>
-      <c r="E20" s="30" t="s">
-        <v>93</v>
+      <c r="E20" s="22" t="s">
+        <v>92</v>
       </c>
       <c r="F20" s="18">
         <v>3</v>
       </c>
-      <c r="G20" s="30" t="s">
-        <v>130</v>
-      </c>
-      <c r="H20" s="30" t="s">
-        <v>160</v>
+      <c r="G20" s="22" t="s">
+        <v>129</v>
+      </c>
+      <c r="H20" s="22" t="s">
+        <v>159</v>
       </c>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.25">
@@ -1830,23 +1841,23 @@
         <v>11</v>
       </c>
       <c r="B21" s="24"/>
-      <c r="C21" s="30" t="s">
+      <c r="C21" s="22" t="s">
         <v>24</v>
       </c>
-      <c r="D21" s="30" t="s">
-        <v>60</v>
-      </c>
-      <c r="E21" s="30" t="s">
-        <v>94</v>
+      <c r="D21" s="22" t="s">
+        <v>59</v>
+      </c>
+      <c r="E21" s="22" t="s">
+        <v>93</v>
       </c>
       <c r="F21" s="18">
         <v>2</v>
       </c>
-      <c r="G21" s="30" t="s">
-        <v>131</v>
-      </c>
-      <c r="H21" s="30" t="s">
-        <v>160</v>
+      <c r="G21" s="22" t="s">
+        <v>130</v>
+      </c>
+      <c r="H21" s="22" t="s">
+        <v>159</v>
       </c>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.25">
@@ -1855,23 +1866,23 @@
         <v>12</v>
       </c>
       <c r="B22" s="24"/>
-      <c r="C22" s="30" t="s">
+      <c r="C22" s="22" t="s">
         <v>25</v>
       </c>
-      <c r="D22" s="30" t="s">
-        <v>61</v>
-      </c>
-      <c r="E22" s="30" t="s">
-        <v>95</v>
+      <c r="D22" s="22" t="s">
+        <v>60</v>
+      </c>
+      <c r="E22" s="22" t="s">
+        <v>94</v>
       </c>
       <c r="F22" s="18">
         <v>2</v>
       </c>
-      <c r="G22" s="30" t="s">
-        <v>132</v>
-      </c>
-      <c r="H22" s="30" t="s">
-        <v>160</v>
+      <c r="G22" s="22" t="s">
+        <v>131</v>
+      </c>
+      <c r="H22" s="22" t="s">
+        <v>159</v>
       </c>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.25">
@@ -1880,23 +1891,23 @@
         <v>13</v>
       </c>
       <c r="B23" s="24"/>
-      <c r="C23" s="30" t="s">
+      <c r="C23" s="22" t="s">
         <v>26</v>
       </c>
-      <c r="D23" s="30" t="s">
-        <v>62</v>
-      </c>
-      <c r="E23" s="30" t="s">
-        <v>96</v>
+      <c r="D23" s="22" t="s">
+        <v>61</v>
+      </c>
+      <c r="E23" s="22" t="s">
+        <v>95</v>
       </c>
       <c r="F23" s="18">
         <v>2</v>
       </c>
-      <c r="G23" s="30" t="s">
-        <v>133</v>
-      </c>
-      <c r="H23" s="30" t="s">
-        <v>160</v>
+      <c r="G23" s="22" t="s">
+        <v>132</v>
+      </c>
+      <c r="H23" s="22" t="s">
+        <v>159</v>
       </c>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.25">
@@ -1905,23 +1916,23 @@
         <v>14</v>
       </c>
       <c r="B24" s="24"/>
-      <c r="C24" s="30" t="s">
+      <c r="C24" s="22" t="s">
         <v>27</v>
       </c>
-      <c r="D24" s="30" t="s">
-        <v>63</v>
-      </c>
-      <c r="E24" s="30" t="s">
-        <v>97</v>
+      <c r="D24" s="22" t="s">
+        <v>62</v>
+      </c>
+      <c r="E24" s="22" t="s">
+        <v>96</v>
       </c>
       <c r="F24" s="18">
         <v>2</v>
       </c>
-      <c r="G24" s="30" t="s">
-        <v>134</v>
-      </c>
-      <c r="H24" s="30" t="s">
-        <v>160</v>
+      <c r="G24" s="22" t="s">
+        <v>133</v>
+      </c>
+      <c r="H24" s="22" t="s">
+        <v>159</v>
       </c>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.25">
@@ -1930,23 +1941,23 @@
         <v>15</v>
       </c>
       <c r="B25" s="24"/>
-      <c r="C25" s="30" t="s">
+      <c r="C25" s="22" t="s">
         <v>28</v>
       </c>
-      <c r="D25" s="30" t="s">
-        <v>64</v>
-      </c>
-      <c r="E25" s="30" t="s">
-        <v>98</v>
+      <c r="D25" s="22" t="s">
+        <v>63</v>
+      </c>
+      <c r="E25" s="22" t="s">
+        <v>97</v>
       </c>
       <c r="F25" s="18">
         <v>2</v>
       </c>
-      <c r="G25" s="30" t="s">
-        <v>135</v>
-      </c>
-      <c r="H25" s="30" t="s">
-        <v>160</v>
+      <c r="G25" s="22" t="s">
+        <v>134</v>
+      </c>
+      <c r="H25" s="22" t="s">
+        <v>159</v>
       </c>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.25">
@@ -1955,23 +1966,23 @@
         <v>16</v>
       </c>
       <c r="B26" s="24"/>
-      <c r="C26" s="30" t="s">
+      <c r="C26" s="22" t="s">
         <v>29</v>
       </c>
-      <c r="D26" s="30" t="s">
-        <v>65</v>
-      </c>
-      <c r="E26" s="30" t="s">
-        <v>99</v>
+      <c r="D26" s="22" t="s">
+        <v>64</v>
+      </c>
+      <c r="E26" s="22" t="s">
+        <v>98</v>
       </c>
       <c r="F26" s="18">
         <v>2</v>
       </c>
-      <c r="G26" s="30" t="s">
-        <v>136</v>
-      </c>
-      <c r="H26" s="30" t="s">
-        <v>160</v>
+      <c r="G26" s="22" t="s">
+        <v>135</v>
+      </c>
+      <c r="H26" s="22" t="s">
+        <v>159</v>
       </c>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.25">
@@ -1980,23 +1991,23 @@
         <v>17</v>
       </c>
       <c r="B27" s="24"/>
-      <c r="C27" s="30" t="s">
+      <c r="C27" s="22" t="s">
         <v>30</v>
       </c>
-      <c r="D27" s="30" t="s">
-        <v>66</v>
-      </c>
-      <c r="E27" s="30" t="s">
-        <v>100</v>
+      <c r="D27" s="22" t="s">
+        <v>65</v>
+      </c>
+      <c r="E27" s="22" t="s">
+        <v>99</v>
       </c>
       <c r="F27" s="18">
         <v>2</v>
       </c>
-      <c r="G27" s="30" t="s">
-        <v>137</v>
-      </c>
-      <c r="H27" s="30" t="s">
-        <v>160</v>
+      <c r="G27" s="22" t="s">
+        <v>136</v>
+      </c>
+      <c r="H27" s="22" t="s">
+        <v>159</v>
       </c>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.25">
@@ -2005,23 +2016,23 @@
         <v>18</v>
       </c>
       <c r="B28" s="24"/>
-      <c r="C28" s="30" t="s">
+      <c r="C28" s="22" t="s">
         <v>31</v>
       </c>
-      <c r="D28" s="30" t="s">
-        <v>67</v>
-      </c>
-      <c r="E28" s="30" t="s">
-        <v>101</v>
+      <c r="D28" s="22" t="s">
+        <v>66</v>
+      </c>
+      <c r="E28" s="22" t="s">
+        <v>100</v>
       </c>
       <c r="F28" s="18">
         <v>2</v>
       </c>
-      <c r="G28" s="30" t="s">
-        <v>138</v>
-      </c>
-      <c r="H28" s="30" t="s">
-        <v>160</v>
+      <c r="G28" s="22" t="s">
+        <v>137</v>
+      </c>
+      <c r="H28" s="22" t="s">
+        <v>159</v>
       </c>
     </row>
     <row r="29" spans="1:8" ht="25.5" x14ac:dyDescent="0.25">
@@ -2030,23 +2041,23 @@
         <v>19</v>
       </c>
       <c r="B29" s="24"/>
-      <c r="C29" s="30" t="s">
+      <c r="C29" s="22" t="s">
         <v>32</v>
       </c>
-      <c r="D29" s="30" t="s">
-        <v>68</v>
-      </c>
-      <c r="E29" s="30" t="s">
-        <v>102</v>
+      <c r="D29" s="22" t="s">
+        <v>67</v>
+      </c>
+      <c r="E29" s="22" t="s">
+        <v>101</v>
       </c>
       <c r="F29" s="18">
         <v>1</v>
       </c>
-      <c r="G29" s="30" t="s">
-        <v>139</v>
-      </c>
-      <c r="H29" s="30" t="s">
-        <v>160</v>
+      <c r="G29" s="22" t="s">
+        <v>138</v>
+      </c>
+      <c r="H29" s="22" t="s">
+        <v>159</v>
       </c>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.25">
@@ -2055,23 +2066,23 @@
         <v>20</v>
       </c>
       <c r="B30" s="24"/>
-      <c r="C30" s="30" t="s">
+      <c r="C30" s="22" t="s">
         <v>33</v>
       </c>
-      <c r="D30" s="30" t="s">
-        <v>69</v>
-      </c>
-      <c r="E30" s="30" t="s">
-        <v>103</v>
+      <c r="D30" s="22" t="s">
+        <v>68</v>
+      </c>
+      <c r="E30" s="22" t="s">
+        <v>102</v>
       </c>
       <c r="F30" s="18">
         <v>1</v>
       </c>
-      <c r="G30" s="30" t="s">
-        <v>140</v>
-      </c>
-      <c r="H30" s="30" t="s">
-        <v>160</v>
+      <c r="G30" s="22" t="s">
+        <v>139</v>
+      </c>
+      <c r="H30" s="22" t="s">
+        <v>159</v>
       </c>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.25">
@@ -2080,23 +2091,23 @@
         <v>21</v>
       </c>
       <c r="B31" s="24"/>
-      <c r="C31" s="30" t="s">
+      <c r="C31" s="22" t="s">
         <v>34</v>
       </c>
-      <c r="D31" s="30" t="s">
-        <v>70</v>
-      </c>
-      <c r="E31" s="30" t="s">
-        <v>104</v>
+      <c r="D31" s="22" t="s">
+        <v>69</v>
+      </c>
+      <c r="E31" s="22" t="s">
+        <v>103</v>
       </c>
       <c r="F31" s="18">
         <v>1</v>
       </c>
-      <c r="G31" s="30" t="s">
-        <v>141</v>
-      </c>
-      <c r="H31" s="30" t="s">
-        <v>160</v>
+      <c r="G31" s="22" t="s">
+        <v>140</v>
+      </c>
+      <c r="H31" s="22" t="s">
+        <v>159</v>
       </c>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.25">
@@ -2105,23 +2116,23 @@
         <v>22</v>
       </c>
       <c r="B32" s="24"/>
-      <c r="C32" s="30" t="s">
+      <c r="C32" s="22" t="s">
         <v>35</v>
       </c>
-      <c r="D32" s="30" t="s">
-        <v>71</v>
-      </c>
-      <c r="E32" s="30" t="s">
-        <v>105</v>
+      <c r="D32" s="22" t="s">
+        <v>70</v>
+      </c>
+      <c r="E32" s="22" t="s">
+        <v>104</v>
       </c>
       <c r="F32" s="18">
         <v>1</v>
       </c>
-      <c r="G32" s="30" t="s">
-        <v>142</v>
-      </c>
-      <c r="H32" s="30" t="s">
-        <v>160</v>
+      <c r="G32" s="22" t="s">
+        <v>141</v>
+      </c>
+      <c r="H32" s="22" t="s">
+        <v>159</v>
       </c>
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.25">
@@ -2130,23 +2141,23 @@
         <v>23</v>
       </c>
       <c r="B33" s="24"/>
-      <c r="C33" s="30" t="s">
+      <c r="C33" s="22" t="s">
         <v>36</v>
       </c>
-      <c r="D33" s="30" t="s">
-        <v>72</v>
-      </c>
-      <c r="E33" s="30" t="s">
-        <v>106</v>
+      <c r="D33" s="22" t="s">
+        <v>71</v>
+      </c>
+      <c r="E33" s="22" t="s">
+        <v>105</v>
       </c>
       <c r="F33" s="18">
         <v>1</v>
       </c>
-      <c r="G33" s="30" t="s">
-        <v>143</v>
-      </c>
-      <c r="H33" s="30" t="s">
-        <v>160</v>
+      <c r="G33" s="22" t="s">
+        <v>142</v>
+      </c>
+      <c r="H33" s="22" t="s">
+        <v>159</v>
       </c>
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.25">
@@ -2155,23 +2166,23 @@
         <v>24</v>
       </c>
       <c r="B34" s="24"/>
-      <c r="C34" s="30" t="s">
+      <c r="C34" s="22" t="s">
         <v>37</v>
       </c>
-      <c r="D34" s="30" t="s">
-        <v>73</v>
-      </c>
-      <c r="E34" s="30" t="s">
-        <v>107</v>
+      <c r="D34" s="22" t="s">
+        <v>72</v>
+      </c>
+      <c r="E34" s="22" t="s">
+        <v>106</v>
       </c>
       <c r="F34" s="18">
         <v>1</v>
       </c>
-      <c r="G34" s="30" t="s">
-        <v>144</v>
-      </c>
-      <c r="H34" s="30" t="s">
-        <v>160</v>
+      <c r="G34" s="22" t="s">
+        <v>143</v>
+      </c>
+      <c r="H34" s="22" t="s">
+        <v>159</v>
       </c>
     </row>
     <row r="35" spans="1:8" ht="25.5" x14ac:dyDescent="0.25">
@@ -2180,23 +2191,23 @@
         <v>25</v>
       </c>
       <c r="B35" s="24"/>
-      <c r="C35" s="30" t="s">
+      <c r="C35" s="22" t="s">
         <v>38</v>
       </c>
-      <c r="D35" s="30" t="s">
-        <v>74</v>
-      </c>
-      <c r="E35" s="30" t="s">
-        <v>108</v>
+      <c r="D35" s="22" t="s">
+        <v>73</v>
+      </c>
+      <c r="E35" s="22" t="s">
+        <v>107</v>
       </c>
       <c r="F35" s="18">
         <v>1</v>
       </c>
-      <c r="G35" s="30" t="s">
-        <v>145</v>
-      </c>
-      <c r="H35" s="30" t="s">
-        <v>160</v>
+      <c r="G35" s="22" t="s">
+        <v>144</v>
+      </c>
+      <c r="H35" s="22" t="s">
+        <v>159</v>
       </c>
     </row>
     <row r="36" spans="1:8" x14ac:dyDescent="0.25">
@@ -2205,23 +2216,23 @@
         <v>26</v>
       </c>
       <c r="B36" s="24"/>
-      <c r="C36" s="30" t="s">
+      <c r="C36" s="22" t="s">
         <v>34</v>
       </c>
-      <c r="D36" s="30" t="s">
-        <v>75</v>
-      </c>
-      <c r="E36" s="30" t="s">
-        <v>109</v>
+      <c r="D36" s="22" t="s">
+        <v>74</v>
+      </c>
+      <c r="E36" s="22" t="s">
+        <v>108</v>
       </c>
       <c r="F36" s="18">
         <v>1</v>
       </c>
-      <c r="G36" s="30" t="s">
-        <v>146</v>
-      </c>
-      <c r="H36" s="30" t="s">
-        <v>160</v>
+      <c r="G36" s="22" t="s">
+        <v>145</v>
+      </c>
+      <c r="H36" s="22" t="s">
+        <v>159</v>
       </c>
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.25">
@@ -2230,23 +2241,23 @@
         <v>27</v>
       </c>
       <c r="B37" s="24"/>
-      <c r="C37" s="30" t="s">
+      <c r="C37" s="22" t="s">
         <v>39</v>
       </c>
-      <c r="D37" s="30" t="s">
-        <v>76</v>
-      </c>
-      <c r="E37" s="30" t="s">
-        <v>110</v>
+      <c r="D37" s="22" t="s">
+        <v>75</v>
+      </c>
+      <c r="E37" s="22" t="s">
+        <v>109</v>
       </c>
       <c r="F37" s="18">
         <v>1</v>
       </c>
-      <c r="G37" s="30" t="s">
-        <v>147</v>
-      </c>
-      <c r="H37" s="30" t="s">
-        <v>160</v>
+      <c r="G37" s="22" t="s">
+        <v>146</v>
+      </c>
+      <c r="H37" s="22" t="s">
+        <v>159</v>
       </c>
     </row>
     <row r="38" spans="1:8" x14ac:dyDescent="0.25">
@@ -2255,23 +2266,23 @@
         <v>28</v>
       </c>
       <c r="B38" s="24"/>
-      <c r="C38" s="30" t="s">
+      <c r="C38" s="22" t="s">
         <v>40</v>
       </c>
-      <c r="D38" s="30" t="s">
-        <v>77</v>
-      </c>
-      <c r="E38" s="30" t="s">
-        <v>111</v>
+      <c r="D38" s="22" t="s">
+        <v>76</v>
+      </c>
+      <c r="E38" s="22" t="s">
+        <v>110</v>
       </c>
       <c r="F38" s="18">
         <v>1</v>
       </c>
-      <c r="G38" s="30" t="s">
-        <v>148</v>
-      </c>
-      <c r="H38" s="30" t="s">
-        <v>160</v>
+      <c r="G38" s="22" t="s">
+        <v>147</v>
+      </c>
+      <c r="H38" s="22" t="s">
+        <v>159</v>
       </c>
     </row>
     <row r="39" spans="1:8" x14ac:dyDescent="0.25">
@@ -2280,23 +2291,23 @@
         <v>29</v>
       </c>
       <c r="B39" s="24"/>
-      <c r="C39" s="30" t="s">
-        <v>41</v>
-      </c>
-      <c r="D39" s="30" t="s">
-        <v>78</v>
-      </c>
-      <c r="E39" s="30" t="s">
-        <v>112</v>
+      <c r="C39" s="22" t="s">
+        <v>160</v>
+      </c>
+      <c r="D39" s="22" t="s">
+        <v>77</v>
+      </c>
+      <c r="E39" s="22" t="s">
+        <v>111</v>
       </c>
       <c r="F39" s="18">
         <v>1</v>
       </c>
-      <c r="G39" s="30" t="s">
-        <v>149</v>
-      </c>
-      <c r="H39" s="30" t="s">
-        <v>160</v>
+      <c r="G39" s="22" t="s">
+        <v>148</v>
+      </c>
+      <c r="H39" s="22" t="s">
+        <v>159</v>
       </c>
     </row>
     <row r="40" spans="1:8" x14ac:dyDescent="0.25">
@@ -2305,23 +2316,23 @@
         <v>30</v>
       </c>
       <c r="B40" s="24"/>
-      <c r="C40" s="30" t="s">
-        <v>41</v>
-      </c>
-      <c r="D40" s="30" t="s">
-        <v>79</v>
-      </c>
-      <c r="E40" s="30" t="s">
-        <v>94</v>
+      <c r="C40" s="22" t="s">
+        <v>162</v>
+      </c>
+      <c r="D40" s="22" t="s">
+        <v>78</v>
+      </c>
+      <c r="E40" s="22" t="s">
+        <v>93</v>
       </c>
       <c r="F40" s="18">
         <v>1</v>
       </c>
-      <c r="G40" s="30" t="s">
-        <v>150</v>
-      </c>
-      <c r="H40" s="30" t="s">
-        <v>160</v>
+      <c r="G40" s="22" t="s">
+        <v>149</v>
+      </c>
+      <c r="H40" s="22" t="s">
+        <v>159</v>
       </c>
     </row>
     <row r="41" spans="1:8" x14ac:dyDescent="0.25">
@@ -2330,23 +2341,23 @@
         <v>31</v>
       </c>
       <c r="B41" s="24"/>
-      <c r="C41" s="30" t="s">
-        <v>41</v>
-      </c>
-      <c r="D41" s="30" t="s">
-        <v>80</v>
-      </c>
-      <c r="E41" s="30" t="s">
-        <v>113</v>
+      <c r="C41" s="22" t="s">
+        <v>161</v>
+      </c>
+      <c r="D41" s="22" t="s">
+        <v>79</v>
+      </c>
+      <c r="E41" s="22" t="s">
+        <v>112</v>
       </c>
       <c r="F41" s="18">
         <v>1</v>
       </c>
-      <c r="G41" s="30" t="s">
-        <v>151</v>
-      </c>
-      <c r="H41" s="30" t="s">
-        <v>160</v>
+      <c r="G41" s="22" t="s">
+        <v>150</v>
+      </c>
+      <c r="H41" s="22" t="s">
+        <v>159</v>
       </c>
     </row>
     <row r="42" spans="1:8" x14ac:dyDescent="0.25">
@@ -2355,23 +2366,23 @@
         <v>32</v>
       </c>
       <c r="B42" s="24"/>
-      <c r="C42" s="30" t="s">
-        <v>42</v>
-      </c>
-      <c r="D42" s="30" t="s">
-        <v>42</v>
-      </c>
-      <c r="E42" s="30" t="s">
-        <v>42</v>
+      <c r="C42" s="22" t="s">
+        <v>41</v>
+      </c>
+      <c r="D42" s="22" t="s">
+        <v>41</v>
+      </c>
+      <c r="E42" s="22" t="s">
+        <v>41</v>
       </c>
       <c r="F42" s="18">
         <v>1</v>
       </c>
-      <c r="G42" s="30" t="s">
-        <v>152</v>
-      </c>
-      <c r="H42" s="30" t="s">
-        <v>160</v>
+      <c r="G42" s="22" t="s">
+        <v>151</v>
+      </c>
+      <c r="H42" s="22" t="s">
+        <v>159</v>
       </c>
     </row>
     <row r="43" spans="1:8" x14ac:dyDescent="0.25">
@@ -2380,23 +2391,23 @@
         <v>33</v>
       </c>
       <c r="B43" s="24"/>
-      <c r="C43" s="30" t="s">
-        <v>43</v>
-      </c>
-      <c r="D43" s="30" t="s">
-        <v>81</v>
-      </c>
-      <c r="E43" s="30" t="s">
-        <v>114</v>
+      <c r="C43" s="22" t="s">
+        <v>42</v>
+      </c>
+      <c r="D43" s="22" t="s">
+        <v>80</v>
+      </c>
+      <c r="E43" s="22" t="s">
+        <v>113</v>
       </c>
       <c r="F43" s="18">
         <v>1</v>
       </c>
-      <c r="G43" s="30" t="s">
-        <v>153</v>
-      </c>
-      <c r="H43" s="30" t="s">
-        <v>160</v>
+      <c r="G43" s="22" t="s">
+        <v>152</v>
+      </c>
+      <c r="H43" s="22" t="s">
+        <v>159</v>
       </c>
     </row>
     <row r="44" spans="1:8" x14ac:dyDescent="0.25">
@@ -2405,23 +2416,23 @@
         <v>34</v>
       </c>
       <c r="B44" s="24"/>
-      <c r="C44" s="30" t="s">
-        <v>44</v>
-      </c>
-      <c r="D44" s="30" t="s">
-        <v>44</v>
-      </c>
-      <c r="E44" s="30" t="s">
-        <v>115</v>
+      <c r="C44" s="22" t="s">
+        <v>43</v>
+      </c>
+      <c r="D44" s="22" t="s">
+        <v>43</v>
+      </c>
+      <c r="E44" s="22" t="s">
+        <v>114</v>
       </c>
       <c r="F44" s="18">
         <v>1</v>
       </c>
-      <c r="G44" s="30" t="s">
-        <v>154</v>
-      </c>
-      <c r="H44" s="30" t="s">
-        <v>160</v>
+      <c r="G44" s="22" t="s">
+        <v>153</v>
+      </c>
+      <c r="H44" s="22" t="s">
+        <v>159</v>
       </c>
     </row>
     <row r="45" spans="1:8" x14ac:dyDescent="0.25">
@@ -2430,23 +2441,23 @@
         <v>35</v>
       </c>
       <c r="B45" s="24"/>
-      <c r="C45" s="30" t="s">
-        <v>45</v>
-      </c>
-      <c r="D45" s="30" t="s">
-        <v>82</v>
-      </c>
-      <c r="E45" s="30" t="s">
-        <v>116</v>
+      <c r="C45" s="22" t="s">
+        <v>44</v>
+      </c>
+      <c r="D45" s="22" t="s">
+        <v>81</v>
+      </c>
+      <c r="E45" s="22" t="s">
+        <v>115</v>
       </c>
       <c r="F45" s="18">
-        <v>1</v>
-      </c>
-      <c r="G45" s="30" t="s">
-        <v>155</v>
-      </c>
-      <c r="H45" s="30" t="s">
-        <v>160</v>
+        <v>2</v>
+      </c>
+      <c r="G45" s="22" t="s">
+        <v>154</v>
+      </c>
+      <c r="H45" s="22" t="s">
+        <v>159</v>
       </c>
     </row>
     <row r="46" spans="1:8" x14ac:dyDescent="0.25">
@@ -2455,23 +2466,23 @@
         <v>36</v>
       </c>
       <c r="B46" s="24"/>
-      <c r="C46" s="30" t="s">
-        <v>46</v>
-      </c>
-      <c r="D46" s="30" t="s">
-        <v>46</v>
-      </c>
-      <c r="E46" s="30" t="s">
-        <v>46</v>
+      <c r="C46" s="22" t="s">
+        <v>45</v>
+      </c>
+      <c r="D46" s="22" t="s">
+        <v>45</v>
+      </c>
+      <c r="E46" s="22" t="s">
+        <v>45</v>
       </c>
       <c r="F46" s="18">
         <v>1</v>
       </c>
-      <c r="G46" s="30" t="s">
-        <v>156</v>
-      </c>
-      <c r="H46" s="30" t="s">
-        <v>160</v>
+      <c r="G46" s="22" t="s">
+        <v>155</v>
+      </c>
+      <c r="H46" s="22" t="s">
+        <v>159</v>
       </c>
     </row>
     <row r="47" spans="1:8" x14ac:dyDescent="0.25">
@@ -2480,23 +2491,23 @@
         <v>37</v>
       </c>
       <c r="B47" s="24"/>
-      <c r="C47" s="30" t="s">
-        <v>47</v>
-      </c>
-      <c r="D47" s="30" t="s">
-        <v>47</v>
-      </c>
-      <c r="E47" s="30" t="s">
-        <v>117</v>
+      <c r="C47" s="22" t="s">
+        <v>46</v>
+      </c>
+      <c r="D47" s="22" t="s">
+        <v>46</v>
+      </c>
+      <c r="E47" s="22" t="s">
+        <v>116</v>
       </c>
       <c r="F47" s="18">
         <v>1</v>
       </c>
-      <c r="G47" s="30" t="s">
-        <v>157</v>
-      </c>
-      <c r="H47" s="30" t="s">
-        <v>160</v>
+      <c r="G47" s="22" t="s">
+        <v>156</v>
+      </c>
+      <c r="H47" s="22" t="s">
+        <v>159</v>
       </c>
     </row>
     <row r="48" spans="1:8" x14ac:dyDescent="0.25">
@@ -2505,23 +2516,23 @@
         <v>38</v>
       </c>
       <c r="B48" s="24"/>
-      <c r="C48" s="30" t="s">
-        <v>48</v>
-      </c>
-      <c r="D48" s="30" t="s">
-        <v>48</v>
-      </c>
-      <c r="E48" s="30" t="s">
-        <v>48</v>
+      <c r="C48" s="22" t="s">
+        <v>47</v>
+      </c>
+      <c r="D48" s="22" t="s">
+        <v>47</v>
+      </c>
+      <c r="E48" s="22" t="s">
+        <v>47</v>
       </c>
       <c r="F48" s="18">
         <v>1</v>
       </c>
-      <c r="G48" s="30" t="s">
-        <v>158</v>
-      </c>
-      <c r="H48" s="30" t="s">
-        <v>160</v>
+      <c r="G48" s="22" t="s">
+        <v>157</v>
+      </c>
+      <c r="H48" s="22" t="s">
+        <v>159</v>
       </c>
     </row>
     <row r="49" spans="1:8" ht="38.25" x14ac:dyDescent="0.25">
@@ -2530,23 +2541,23 @@
         <v>39</v>
       </c>
       <c r="B49" s="24"/>
-      <c r="C49" s="30" t="s">
-        <v>49</v>
-      </c>
-      <c r="D49" s="30" t="s">
-        <v>49</v>
-      </c>
-      <c r="E49" s="30" t="s">
-        <v>118</v>
+      <c r="C49" s="22" t="s">
+        <v>48</v>
+      </c>
+      <c r="D49" s="22" t="s">
+        <v>48</v>
+      </c>
+      <c r="E49" s="22" t="s">
+        <v>117</v>
       </c>
       <c r="F49" s="18">
         <v>1</v>
       </c>
-      <c r="G49" s="30" t="s">
-        <v>159</v>
-      </c>
-      <c r="H49" s="30" t="s">
-        <v>160</v>
+      <c r="G49" s="22" t="s">
+        <v>158</v>
+      </c>
+      <c r="H49" s="22" t="s">
+        <v>159</v>
       </c>
     </row>
     <row r="50" spans="1:8" x14ac:dyDescent="0.25">
@@ -2698,36 +2709,6 @@
   </sheetData>
   <autoFilter ref="C10:H10" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
   <mergeCells count="46">
-    <mergeCell ref="A44:B44"/>
-    <mergeCell ref="A45:B45"/>
-    <mergeCell ref="A46:B46"/>
-    <mergeCell ref="A47:B47"/>
-    <mergeCell ref="A48:B48"/>
-    <mergeCell ref="A39:B39"/>
-    <mergeCell ref="A40:B40"/>
-    <mergeCell ref="A41:B41"/>
-    <mergeCell ref="A42:B42"/>
-    <mergeCell ref="A43:B43"/>
-    <mergeCell ref="A34:B34"/>
-    <mergeCell ref="A35:B35"/>
-    <mergeCell ref="A36:B36"/>
-    <mergeCell ref="A37:B37"/>
-    <mergeCell ref="A38:B38"/>
-    <mergeCell ref="A29:B29"/>
-    <mergeCell ref="A30:B30"/>
-    <mergeCell ref="A31:B31"/>
-    <mergeCell ref="A32:B32"/>
-    <mergeCell ref="A33:B33"/>
-    <mergeCell ref="A24:B24"/>
-    <mergeCell ref="A25:B25"/>
-    <mergeCell ref="A26:B26"/>
-    <mergeCell ref="A27:B27"/>
-    <mergeCell ref="A28:B28"/>
-    <mergeCell ref="C1:H1"/>
-    <mergeCell ref="D2:H2"/>
-    <mergeCell ref="D3:H3"/>
-    <mergeCell ref="D4:H4"/>
-    <mergeCell ref="D5:H5"/>
     <mergeCell ref="A10:B10"/>
     <mergeCell ref="A11:B11"/>
     <mergeCell ref="A12:B12"/>
@@ -2744,6 +2725,36 @@
     <mergeCell ref="A21:B21"/>
     <mergeCell ref="A22:B22"/>
     <mergeCell ref="A23:B23"/>
+    <mergeCell ref="C1:H1"/>
+    <mergeCell ref="D2:H2"/>
+    <mergeCell ref="D3:H3"/>
+    <mergeCell ref="D4:H4"/>
+    <mergeCell ref="D5:H5"/>
+    <mergeCell ref="A24:B24"/>
+    <mergeCell ref="A25:B25"/>
+    <mergeCell ref="A26:B26"/>
+    <mergeCell ref="A27:B27"/>
+    <mergeCell ref="A28:B28"/>
+    <mergeCell ref="A29:B29"/>
+    <mergeCell ref="A30:B30"/>
+    <mergeCell ref="A31:B31"/>
+    <mergeCell ref="A32:B32"/>
+    <mergeCell ref="A33:B33"/>
+    <mergeCell ref="A34:B34"/>
+    <mergeCell ref="A35:B35"/>
+    <mergeCell ref="A36:B36"/>
+    <mergeCell ref="A37:B37"/>
+    <mergeCell ref="A38:B38"/>
+    <mergeCell ref="A39:B39"/>
+    <mergeCell ref="A40:B40"/>
+    <mergeCell ref="A41:B41"/>
+    <mergeCell ref="A42:B42"/>
+    <mergeCell ref="A43:B43"/>
+    <mergeCell ref="A44:B44"/>
+    <mergeCell ref="A45:B45"/>
+    <mergeCell ref="A46:B46"/>
+    <mergeCell ref="A47:B47"/>
+    <mergeCell ref="A48:B48"/>
   </mergeCells>
   <conditionalFormatting sqref="H11:H12">
     <cfRule type="cellIs" dxfId="37" priority="38" operator="equal">

</xml_diff>

<commit_message>
hardware: outputs: Updating all output files for release v0.7 #258
</commit_message>
<xml_diff>
--- a/hardware/outputs/board_bom/board_bom.xlsx
+++ b/hardware/outputs/board_bom/board_bom.xlsx
@@ -3,9 +3,14 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24026"/>
   <workbookPr/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{8562DC8D-57E0-40EA-826C-6DD3DA10F1CD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Yan Azeredo\Desktop\SpaceLab\obdh2\hardware\outputs\board_bom\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1AD70765-1E12-4F0C-B013-DAC29E261758}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2250" yWindow="2250" windowWidth="15375" windowHeight="7875" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Plan1" sheetId="1" r:id="rId1"/>
@@ -759,6 +764,15 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -768,20 +782,11 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1404,8 +1409,8 @@
   </sheetPr>
   <dimension ref="A1:M71"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageBreakPreview" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="A40" zoomScale="85" zoomScaleNormal="100" zoomScaleSheetLayoutView="85" workbookViewId="0">
+      <selection activeCell="C49" sqref="C49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1428,11 +1433,11 @@
       <c r="A1" s="1"/>
       <c r="B1" s="17"/>
       <c r="C1" s="17"/>
-      <c r="D1" s="24" t="s">
+      <c r="D1" s="27" t="s">
         <v>6</v>
       </c>
-      <c r="E1" s="25"/>
-      <c r="F1" s="26"/>
+      <c r="E1" s="28"/>
+      <c r="F1" s="29"/>
       <c r="G1" s="18"/>
       <c r="H1" s="18"/>
       <c r="I1" s="18"/>
@@ -1448,10 +1453,10 @@
       <c r="D2" s="21" t="s">
         <v>0</v>
       </c>
-      <c r="E2" s="28" t="s">
+      <c r="E2" s="30" t="s">
         <v>8</v>
       </c>
-      <c r="F2" s="27"/>
+      <c r="F2" s="31"/>
       <c r="G2" s="20"/>
       <c r="H2" s="20"/>
       <c r="I2" s="20"/>
@@ -1467,10 +1472,10 @@
       <c r="D3" s="21" t="s">
         <v>1</v>
       </c>
-      <c r="E3" s="28" t="s">
+      <c r="E3" s="30" t="s">
         <v>8</v>
       </c>
-      <c r="F3" s="27"/>
+      <c r="F3" s="31"/>
       <c r="G3" s="20"/>
       <c r="H3" s="20"/>
       <c r="I3" s="20"/>
@@ -1486,10 +1491,10 @@
       <c r="D4" s="21" t="s">
         <v>2</v>
       </c>
-      <c r="E4" s="28" t="s">
+      <c r="E4" s="30" t="s">
         <v>9</v>
       </c>
-      <c r="F4" s="27"/>
+      <c r="F4" s="31"/>
       <c r="G4" s="19"/>
       <c r="H4" s="20"/>
       <c r="I4" s="20"/>
@@ -1505,10 +1510,10 @@
       <c r="D5" s="21" t="s">
         <v>7</v>
       </c>
-      <c r="E5" s="28" t="s">
+      <c r="E5" s="30" t="s">
         <v>10</v>
       </c>
-      <c r="F5" s="27"/>
+      <c r="F5" s="31"/>
       <c r="G5" s="20"/>
       <c r="H5" s="20"/>
       <c r="I5" s="20"/>
@@ -1524,10 +1529,10 @@
       <c r="D6" s="22" t="s">
         <v>3</v>
       </c>
-      <c r="E6" s="29" t="s">
+      <c r="E6" s="24" t="s">
         <v>11</v>
       </c>
-      <c r="F6" s="29" t="s">
+      <c r="F6" s="24" t="s">
         <v>12</v>
       </c>
       <c r="G6" s="20"/>
@@ -1547,11 +1552,11 @@
       </c>
       <c r="E7" s="7">
         <f ca="1">TODAY()</f>
-        <v>44351</v>
+        <v>44354</v>
       </c>
       <c r="F7" s="8">
         <f ca="1">NOW()</f>
-        <v>44351.691632407405</v>
+        <v>44354.912312152781</v>
       </c>
       <c r="G7" s="20"/>
       <c r="H7" s="20"/>
@@ -1632,66 +1637,66 @@
         <f>ROW(A11) - ROW($A$10)</f>
         <v>1</v>
       </c>
-      <c r="B11" s="30" t="s">
+      <c r="B11" s="25" t="s">
         <v>14</v>
       </c>
       <c r="C11" s="14">
         <v>24</v>
       </c>
-      <c r="D11" s="30" t="s">
-        <v>57</v>
-      </c>
-      <c r="E11" s="30" t="s">
-        <v>57</v>
-      </c>
-      <c r="F11" s="30" t="s">
+      <c r="D11" s="25" t="s">
+        <v>57</v>
+      </c>
+      <c r="E11" s="25" t="s">
+        <v>57</v>
+      </c>
+      <c r="F11" s="25" t="s">
         <v>63</v>
       </c>
-      <c r="G11" s="31" t="s">
+      <c r="G11" s="26" t="s">
         <v>104</v>
       </c>
       <c r="H11" s="15"/>
-      <c r="I11" s="31" t="s">
+      <c r="I11" s="26" t="s">
         <v>143</v>
       </c>
-      <c r="J11" s="31" t="s">
-        <v>57</v>
-      </c>
-      <c r="K11" s="31" t="s">
+      <c r="J11" s="26" t="s">
+        <v>57</v>
+      </c>
+      <c r="K11" s="26" t="s">
         <v>167</v>
       </c>
     </row>
     <row r="12" spans="1:13" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A12" s="14">
-        <f t="shared" ref="A12:A51" si="0">ROW(A12) - ROW($A$10)</f>
+        <f t="shared" ref="A12:A50" si="0">ROW(A12) - ROW($A$10)</f>
         <v>2</v>
       </c>
-      <c r="B12" s="30" t="s">
+      <c r="B12" s="25" t="s">
         <v>15</v>
       </c>
       <c r="C12" s="14">
         <v>17</v>
       </c>
-      <c r="D12" s="30" t="s">
-        <v>57</v>
-      </c>
-      <c r="E12" s="30" t="s">
-        <v>57</v>
-      </c>
-      <c r="F12" s="30" t="s">
+      <c r="D12" s="25" t="s">
+        <v>57</v>
+      </c>
+      <c r="E12" s="25" t="s">
+        <v>57</v>
+      </c>
+      <c r="F12" s="25" t="s">
         <v>64</v>
       </c>
-      <c r="G12" s="31" t="s">
+      <c r="G12" s="26" t="s">
         <v>105</v>
       </c>
       <c r="H12" s="15"/>
-      <c r="I12" s="31" t="s">
+      <c r="I12" s="26" t="s">
         <v>143</v>
       </c>
-      <c r="J12" s="31" t="s">
-        <v>57</v>
-      </c>
-      <c r="K12" s="31" t="s">
+      <c r="J12" s="26" t="s">
+        <v>57</v>
+      </c>
+      <c r="K12" s="26" t="s">
         <v>167</v>
       </c>
     </row>
@@ -1700,32 +1705,32 @@
         <f>ROW(A13) - ROW($A$10)</f>
         <v>3</v>
       </c>
-      <c r="B13" s="30" t="s">
+      <c r="B13" s="25" t="s">
         <v>16</v>
       </c>
       <c r="C13" s="14">
         <v>14</v>
       </c>
-      <c r="D13" s="30" t="s">
-        <v>57</v>
-      </c>
-      <c r="E13" s="30" t="s">
-        <v>57</v>
-      </c>
-      <c r="F13" s="30" t="s">
+      <c r="D13" s="25" t="s">
+        <v>57</v>
+      </c>
+      <c r="E13" s="25" t="s">
+        <v>57</v>
+      </c>
+      <c r="F13" s="25" t="s">
         <v>65</v>
       </c>
-      <c r="G13" s="31" t="s">
+      <c r="G13" s="26" t="s">
         <v>106</v>
       </c>
       <c r="H13" s="15"/>
-      <c r="I13" s="31" t="s">
+      <c r="I13" s="26" t="s">
         <v>144</v>
       </c>
-      <c r="J13" s="31" t="s">
-        <v>57</v>
-      </c>
-      <c r="K13" s="31" t="s">
+      <c r="J13" s="26" t="s">
+        <v>57</v>
+      </c>
+      <c r="K13" s="26" t="s">
         <v>167</v>
       </c>
     </row>
@@ -1734,32 +1739,32 @@
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
-      <c r="B14" s="30" t="s">
+      <c r="B14" s="25" t="s">
         <v>17</v>
       </c>
       <c r="C14" s="14">
         <v>8</v>
       </c>
-      <c r="D14" s="30" t="s">
-        <v>57</v>
-      </c>
-      <c r="E14" s="30" t="s">
-        <v>57</v>
-      </c>
-      <c r="F14" s="30" t="s">
+      <c r="D14" s="25" t="s">
+        <v>57</v>
+      </c>
+      <c r="E14" s="25" t="s">
+        <v>57</v>
+      </c>
+      <c r="F14" s="25" t="s">
         <v>66</v>
       </c>
-      <c r="G14" s="31" t="s">
+      <c r="G14" s="26" t="s">
         <v>107</v>
       </c>
       <c r="H14" s="15"/>
-      <c r="I14" s="31" t="s">
+      <c r="I14" s="26" t="s">
         <v>143</v>
       </c>
-      <c r="J14" s="31" t="s">
-        <v>57</v>
-      </c>
-      <c r="K14" s="31" t="s">
+      <c r="J14" s="26" t="s">
+        <v>57</v>
+      </c>
+      <c r="K14" s="26" t="s">
         <v>167</v>
       </c>
     </row>
@@ -1768,32 +1773,32 @@
         <f>ROW(A15) - ROW($A$10)</f>
         <v>5</v>
       </c>
-      <c r="B15" s="30" t="s">
+      <c r="B15" s="25" t="s">
         <v>18</v>
       </c>
       <c r="C15" s="14">
         <v>7</v>
       </c>
-      <c r="D15" s="30" t="s">
-        <v>57</v>
-      </c>
-      <c r="E15" s="30" t="s">
-        <v>57</v>
-      </c>
-      <c r="F15" s="30" t="s">
+      <c r="D15" s="25" t="s">
+        <v>57</v>
+      </c>
+      <c r="E15" s="25" t="s">
+        <v>57</v>
+      </c>
+      <c r="F15" s="25" t="s">
         <v>67</v>
       </c>
-      <c r="G15" s="31" t="s">
+      <c r="G15" s="26" t="s">
         <v>108</v>
       </c>
       <c r="H15" s="15"/>
-      <c r="I15" s="31" t="s">
+      <c r="I15" s="26" t="s">
         <v>143</v>
       </c>
-      <c r="J15" s="31" t="s">
-        <v>57</v>
-      </c>
-      <c r="K15" s="31" t="s">
+      <c r="J15" s="26" t="s">
+        <v>57</v>
+      </c>
+      <c r="K15" s="26" t="s">
         <v>167</v>
       </c>
     </row>
@@ -1802,32 +1807,32 @@
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
-      <c r="B16" s="30" t="s">
+      <c r="B16" s="25" t="s">
         <v>19</v>
       </c>
       <c r="C16" s="14">
         <v>6</v>
       </c>
-      <c r="D16" s="30" t="s">
-        <v>57</v>
-      </c>
-      <c r="E16" s="30" t="s">
-        <v>57</v>
-      </c>
-      <c r="F16" s="30" t="s">
+      <c r="D16" s="25" t="s">
+        <v>57</v>
+      </c>
+      <c r="E16" s="25" t="s">
+        <v>57</v>
+      </c>
+      <c r="F16" s="25" t="s">
         <v>68</v>
       </c>
-      <c r="G16" s="31" t="s">
+      <c r="G16" s="26" t="s">
         <v>109</v>
       </c>
       <c r="H16" s="15"/>
-      <c r="I16" s="31" t="s">
+      <c r="I16" s="26" t="s">
         <v>145</v>
       </c>
-      <c r="J16" s="31" t="s">
-        <v>57</v>
-      </c>
-      <c r="K16" s="31" t="s">
+      <c r="J16" s="26" t="s">
+        <v>57</v>
+      </c>
+      <c r="K16" s="26" t="s">
         <v>167</v>
       </c>
     </row>
@@ -1836,32 +1841,32 @@
         <f>ROW(A17) - ROW($A$10)</f>
         <v>7</v>
       </c>
-      <c r="B17" s="30" t="s">
+      <c r="B17" s="25" t="s">
         <v>20</v>
       </c>
       <c r="C17" s="14">
         <v>4</v>
       </c>
-      <c r="D17" s="30" t="s">
-        <v>57</v>
-      </c>
-      <c r="E17" s="30" t="s">
-        <v>57</v>
-      </c>
-      <c r="F17" s="30" t="s">
+      <c r="D17" s="25" t="s">
+        <v>57</v>
+      </c>
+      <c r="E17" s="25" t="s">
+        <v>57</v>
+      </c>
+      <c r="F17" s="25" t="s">
         <v>69</v>
       </c>
-      <c r="G17" s="31" t="s">
+      <c r="G17" s="26" t="s">
         <v>110</v>
       </c>
       <c r="H17" s="15"/>
-      <c r="I17" s="31" t="s">
+      <c r="I17" s="26" t="s">
         <v>144</v>
       </c>
-      <c r="J17" s="31" t="s">
-        <v>57</v>
-      </c>
-      <c r="K17" s="31" t="s">
+      <c r="J17" s="26" t="s">
+        <v>57</v>
+      </c>
+      <c r="K17" s="26" t="s">
         <v>167</v>
       </c>
     </row>
@@ -1870,32 +1875,32 @@
         <f t="shared" si="0"/>
         <v>8</v>
       </c>
-      <c r="B18" s="30" t="s">
+      <c r="B18" s="25" t="s">
         <v>21</v>
       </c>
       <c r="C18" s="14">
         <v>4</v>
       </c>
-      <c r="D18" s="30" t="s">
-        <v>57</v>
-      </c>
-      <c r="E18" s="30" t="s">
-        <v>57</v>
-      </c>
-      <c r="F18" s="30" t="s">
+      <c r="D18" s="25" t="s">
+        <v>57</v>
+      </c>
+      <c r="E18" s="25" t="s">
+        <v>57</v>
+      </c>
+      <c r="F18" s="25" t="s">
         <v>70</v>
       </c>
-      <c r="G18" s="31" t="s">
+      <c r="G18" s="26" t="s">
         <v>111</v>
       </c>
       <c r="H18" s="15"/>
-      <c r="I18" s="31" t="s">
+      <c r="I18" s="26" t="s">
         <v>146</v>
       </c>
-      <c r="J18" s="31" t="s">
-        <v>57</v>
-      </c>
-      <c r="K18" s="31" t="s">
+      <c r="J18" s="26" t="s">
+        <v>57</v>
+      </c>
+      <c r="K18" s="26" t="s">
         <v>167</v>
       </c>
     </row>
@@ -1904,32 +1909,32 @@
         <f>ROW(A19) - ROW($A$10)</f>
         <v>9</v>
       </c>
-      <c r="B19" s="30" t="s">
+      <c r="B19" s="25" t="s">
         <v>22</v>
       </c>
       <c r="C19" s="14">
         <v>4</v>
       </c>
-      <c r="D19" s="30" t="s">
-        <v>57</v>
-      </c>
-      <c r="E19" s="30" t="s">
-        <v>57</v>
-      </c>
-      <c r="F19" s="30" t="s">
+      <c r="D19" s="25" t="s">
+        <v>57</v>
+      </c>
+      <c r="E19" s="25" t="s">
+        <v>57</v>
+      </c>
+      <c r="F19" s="25" t="s">
         <v>71</v>
       </c>
-      <c r="G19" s="31" t="s">
+      <c r="G19" s="26" t="s">
         <v>112</v>
       </c>
       <c r="H19" s="15"/>
-      <c r="I19" s="31" t="s">
+      <c r="I19" s="26" t="s">
         <v>146</v>
       </c>
-      <c r="J19" s="31" t="s">
-        <v>57</v>
-      </c>
-      <c r="K19" s="31" t="s">
+      <c r="J19" s="26" t="s">
+        <v>57</v>
+      </c>
+      <c r="K19" s="26" t="s">
         <v>167</v>
       </c>
     </row>
@@ -1938,32 +1943,32 @@
         <f t="shared" si="0"/>
         <v>10</v>
       </c>
-      <c r="B20" s="30" t="s">
+      <c r="B20" s="25" t="s">
         <v>23</v>
       </c>
       <c r="C20" s="14">
         <v>3</v>
       </c>
-      <c r="D20" s="30" t="s">
-        <v>57</v>
-      </c>
-      <c r="E20" s="30" t="s">
-        <v>57</v>
-      </c>
-      <c r="F20" s="30" t="s">
+      <c r="D20" s="25" t="s">
+        <v>57</v>
+      </c>
+      <c r="E20" s="25" t="s">
+        <v>57</v>
+      </c>
+      <c r="F20" s="25" t="s">
         <v>72</v>
       </c>
-      <c r="G20" s="31" t="s">
+      <c r="G20" s="26" t="s">
         <v>113</v>
       </c>
       <c r="H20" s="15"/>
-      <c r="I20" s="31" t="s">
+      <c r="I20" s="26" t="s">
         <v>147</v>
       </c>
-      <c r="J20" s="31" t="s">
-        <v>57</v>
-      </c>
-      <c r="K20" s="31" t="s">
+      <c r="J20" s="26" t="s">
+        <v>57</v>
+      </c>
+      <c r="K20" s="26" t="s">
         <v>167</v>
       </c>
     </row>
@@ -1972,32 +1977,32 @@
         <f>ROW(A21) - ROW($A$10)</f>
         <v>11</v>
       </c>
-      <c r="B21" s="30" t="s">
+      <c r="B21" s="25" t="s">
         <v>24</v>
       </c>
       <c r="C21" s="14">
         <v>2</v>
       </c>
-      <c r="D21" s="30" t="s">
-        <v>57</v>
-      </c>
-      <c r="E21" s="30" t="s">
-        <v>57</v>
-      </c>
-      <c r="F21" s="30" t="s">
+      <c r="D21" s="25" t="s">
+        <v>57</v>
+      </c>
+      <c r="E21" s="25" t="s">
+        <v>57</v>
+      </c>
+      <c r="F21" s="25" t="s">
         <v>73</v>
       </c>
-      <c r="G21" s="31" t="s">
+      <c r="G21" s="26" t="s">
         <v>114</v>
       </c>
       <c r="H21" s="15"/>
-      <c r="I21" s="31" t="s">
+      <c r="I21" s="26" t="s">
         <v>144</v>
       </c>
-      <c r="J21" s="31" t="s">
-        <v>57</v>
-      </c>
-      <c r="K21" s="31" t="s">
+      <c r="J21" s="26" t="s">
+        <v>57</v>
+      </c>
+      <c r="K21" s="26" t="s">
         <v>167</v>
       </c>
     </row>
@@ -2006,32 +2011,32 @@
         <f t="shared" si="0"/>
         <v>12</v>
       </c>
-      <c r="B22" s="30" t="s">
+      <c r="B22" s="25" t="s">
         <v>25</v>
       </c>
       <c r="C22" s="14">
         <v>2</v>
       </c>
-      <c r="D22" s="30" t="s">
-        <v>57</v>
-      </c>
-      <c r="E22" s="30" t="s">
-        <v>57</v>
-      </c>
-      <c r="F22" s="30" t="s">
+      <c r="D22" s="25" t="s">
+        <v>57</v>
+      </c>
+      <c r="E22" s="25" t="s">
+        <v>57</v>
+      </c>
+      <c r="F22" s="25" t="s">
         <v>74</v>
       </c>
-      <c r="G22" s="31" t="s">
+      <c r="G22" s="26" t="s">
         <v>115</v>
       </c>
       <c r="H22" s="15"/>
-      <c r="I22" s="31" t="s">
+      <c r="I22" s="26" t="s">
         <v>144</v>
       </c>
-      <c r="J22" s="31" t="s">
-        <v>57</v>
-      </c>
-      <c r="K22" s="31" t="s">
+      <c r="J22" s="26" t="s">
+        <v>57</v>
+      </c>
+      <c r="K22" s="26" t="s">
         <v>167</v>
       </c>
     </row>
@@ -2040,32 +2045,32 @@
         <f>ROW(A23) - ROW($A$10)</f>
         <v>13</v>
       </c>
-      <c r="B23" s="30" t="s">
+      <c r="B23" s="25" t="s">
         <v>26</v>
       </c>
       <c r="C23" s="14">
         <v>2</v>
       </c>
-      <c r="D23" s="30" t="s">
-        <v>57</v>
-      </c>
-      <c r="E23" s="30" t="s">
-        <v>57</v>
-      </c>
-      <c r="F23" s="30" t="s">
+      <c r="D23" s="25" t="s">
+        <v>57</v>
+      </c>
+      <c r="E23" s="25" t="s">
+        <v>57</v>
+      </c>
+      <c r="F23" s="25" t="s">
         <v>75</v>
       </c>
-      <c r="G23" s="31" t="s">
+      <c r="G23" s="26" t="s">
         <v>116</v>
       </c>
       <c r="H23" s="15"/>
-      <c r="I23" s="31" t="s">
+      <c r="I23" s="26" t="s">
         <v>143</v>
       </c>
-      <c r="J23" s="31" t="s">
-        <v>57</v>
-      </c>
-      <c r="K23" s="31" t="s">
+      <c r="J23" s="26" t="s">
+        <v>57</v>
+      </c>
+      <c r="K23" s="26" t="s">
         <v>167</v>
       </c>
     </row>
@@ -2074,32 +2079,32 @@
         <f t="shared" si="0"/>
         <v>14</v>
       </c>
-      <c r="B24" s="30" t="s">
+      <c r="B24" s="25" t="s">
         <v>27</v>
       </c>
       <c r="C24" s="14">
         <v>2</v>
       </c>
-      <c r="D24" s="30" t="s">
-        <v>57</v>
-      </c>
-      <c r="E24" s="30" t="s">
-        <v>57</v>
-      </c>
-      <c r="F24" s="30" t="s">
+      <c r="D24" s="25" t="s">
+        <v>57</v>
+      </c>
+      <c r="E24" s="25" t="s">
+        <v>57</v>
+      </c>
+      <c r="F24" s="25" t="s">
         <v>76</v>
       </c>
-      <c r="G24" s="31" t="s">
+      <c r="G24" s="26" t="s">
         <v>117</v>
       </c>
       <c r="H24" s="15"/>
-      <c r="I24" s="31" t="s">
+      <c r="I24" s="26" t="s">
         <v>144</v>
       </c>
-      <c r="J24" s="31" t="s">
-        <v>57</v>
-      </c>
-      <c r="K24" s="31" t="s">
+      <c r="J24" s="26" t="s">
+        <v>57</v>
+      </c>
+      <c r="K24" s="26" t="s">
         <v>167</v>
       </c>
     </row>
@@ -2108,32 +2113,32 @@
         <f>ROW(A25) - ROW($A$10)</f>
         <v>15</v>
       </c>
-      <c r="B25" s="30" t="s">
+      <c r="B25" s="25" t="s">
         <v>28</v>
       </c>
       <c r="C25" s="14">
         <v>2</v>
       </c>
-      <c r="D25" s="30" t="s">
-        <v>57</v>
-      </c>
-      <c r="E25" s="30" t="s">
-        <v>57</v>
-      </c>
-      <c r="F25" s="30" t="s">
+      <c r="D25" s="25" t="s">
+        <v>57</v>
+      </c>
+      <c r="E25" s="25" t="s">
+        <v>57</v>
+      </c>
+      <c r="F25" s="25" t="s">
         <v>77</v>
       </c>
-      <c r="G25" s="31" t="s">
+      <c r="G25" s="26" t="s">
         <v>118</v>
       </c>
       <c r="H25" s="15"/>
-      <c r="I25" s="31" t="s">
+      <c r="I25" s="26" t="s">
         <v>148</v>
       </c>
-      <c r="J25" s="31" t="s">
-        <v>57</v>
-      </c>
-      <c r="K25" s="31" t="s">
+      <c r="J25" s="26" t="s">
+        <v>57</v>
+      </c>
+      <c r="K25" s="26" t="s">
         <v>167</v>
       </c>
     </row>
@@ -2142,32 +2147,32 @@
         <f t="shared" si="0"/>
         <v>16</v>
       </c>
-      <c r="B26" s="30" t="s">
+      <c r="B26" s="25" t="s">
         <v>29</v>
       </c>
       <c r="C26" s="14">
         <v>2</v>
       </c>
-      <c r="D26" s="30" t="s">
-        <v>57</v>
-      </c>
-      <c r="E26" s="30" t="s">
-        <v>57</v>
-      </c>
-      <c r="F26" s="30" t="s">
+      <c r="D26" s="25" t="s">
+        <v>57</v>
+      </c>
+      <c r="E26" s="25" t="s">
+        <v>57</v>
+      </c>
+      <c r="F26" s="25" t="s">
         <v>78</v>
       </c>
-      <c r="G26" s="31" t="s">
+      <c r="G26" s="26" t="s">
         <v>119</v>
       </c>
       <c r="H26" s="15"/>
-      <c r="I26" s="31" t="s">
+      <c r="I26" s="26" t="s">
         <v>149</v>
       </c>
-      <c r="J26" s="31" t="s">
-        <v>57</v>
-      </c>
-      <c r="K26" s="31" t="s">
+      <c r="J26" s="26" t="s">
+        <v>57</v>
+      </c>
+      <c r="K26" s="26" t="s">
         <v>167</v>
       </c>
     </row>
@@ -2176,32 +2181,32 @@
         <f>ROW(A27) - ROW($A$10)</f>
         <v>17</v>
       </c>
-      <c r="B27" s="30" t="s">
+      <c r="B27" s="25" t="s">
         <v>30</v>
       </c>
       <c r="C27" s="14">
         <v>2</v>
       </c>
-      <c r="D27" s="30" t="s">
-        <v>57</v>
-      </c>
-      <c r="E27" s="30" t="s">
-        <v>57</v>
-      </c>
-      <c r="F27" s="30" t="s">
+      <c r="D27" s="25" t="s">
+        <v>57</v>
+      </c>
+      <c r="E27" s="25" t="s">
+        <v>57</v>
+      </c>
+      <c r="F27" s="25" t="s">
         <v>79</v>
       </c>
-      <c r="G27" s="31" t="s">
+      <c r="G27" s="26" t="s">
         <v>120</v>
       </c>
       <c r="H27" s="15"/>
-      <c r="I27" s="31" t="s">
+      <c r="I27" s="26" t="s">
         <v>144</v>
       </c>
-      <c r="J27" s="31" t="s">
-        <v>57</v>
-      </c>
-      <c r="K27" s="31" t="s">
+      <c r="J27" s="26" t="s">
+        <v>57</v>
+      </c>
+      <c r="K27" s="26" t="s">
         <v>167</v>
       </c>
     </row>
@@ -2210,32 +2215,32 @@
         <f t="shared" si="0"/>
         <v>18</v>
       </c>
-      <c r="B28" s="30" t="s">
+      <c r="B28" s="25" t="s">
         <v>31</v>
       </c>
       <c r="C28" s="14">
         <v>2</v>
       </c>
-      <c r="D28" s="30" t="s">
-        <v>57</v>
-      </c>
-      <c r="E28" s="30" t="s">
-        <v>57</v>
-      </c>
-      <c r="F28" s="30" t="s">
+      <c r="D28" s="25" t="s">
+        <v>57</v>
+      </c>
+      <c r="E28" s="25" t="s">
+        <v>57</v>
+      </c>
+      <c r="F28" s="25" t="s">
         <v>80</v>
       </c>
-      <c r="G28" s="31" t="s">
+      <c r="G28" s="26" t="s">
         <v>121</v>
       </c>
       <c r="H28" s="15"/>
-      <c r="I28" s="31" t="s">
+      <c r="I28" s="26" t="s">
         <v>143</v>
       </c>
-      <c r="J28" s="31" t="s">
-        <v>57</v>
-      </c>
-      <c r="K28" s="31" t="s">
+      <c r="J28" s="26" t="s">
+        <v>57</v>
+      </c>
+      <c r="K28" s="26" t="s">
         <v>167</v>
       </c>
     </row>
@@ -2244,32 +2249,32 @@
         <f>ROW(A29) - ROW($A$10)</f>
         <v>19</v>
       </c>
-      <c r="B29" s="30" t="s">
+      <c r="B29" s="25" t="s">
         <v>32</v>
       </c>
       <c r="C29" s="14">
         <v>2</v>
       </c>
-      <c r="D29" s="30" t="s">
-        <v>57</v>
-      </c>
-      <c r="E29" s="30" t="s">
-        <v>57</v>
-      </c>
-      <c r="F29" s="30" t="s">
+      <c r="D29" s="25" t="s">
+        <v>57</v>
+      </c>
+      <c r="E29" s="25" t="s">
+        <v>57</v>
+      </c>
+      <c r="F29" s="25" t="s">
         <v>81</v>
       </c>
-      <c r="G29" s="31" t="s">
+      <c r="G29" s="26" t="s">
         <v>122</v>
       </c>
       <c r="H29" s="15"/>
-      <c r="I29" s="31" t="s">
+      <c r="I29" s="26" t="s">
         <v>150</v>
       </c>
-      <c r="J29" s="31" t="s">
-        <v>57</v>
-      </c>
-      <c r="K29" s="31" t="s">
+      <c r="J29" s="26" t="s">
+        <v>57</v>
+      </c>
+      <c r="K29" s="26" t="s">
         <v>167</v>
       </c>
     </row>
@@ -2278,32 +2283,32 @@
         <f t="shared" si="0"/>
         <v>20</v>
       </c>
-      <c r="B30" s="30" t="s">
+      <c r="B30" s="25" t="s">
         <v>33</v>
       </c>
       <c r="C30" s="14">
         <v>2</v>
       </c>
-      <c r="D30" s="30" t="s">
-        <v>57</v>
-      </c>
-      <c r="E30" s="30" t="s">
-        <v>57</v>
-      </c>
-      <c r="F30" s="30" t="s">
+      <c r="D30" s="25" t="s">
+        <v>57</v>
+      </c>
+      <c r="E30" s="25" t="s">
+        <v>57</v>
+      </c>
+      <c r="F30" s="25" t="s">
         <v>82</v>
       </c>
-      <c r="G30" s="31" t="s">
+      <c r="G30" s="26" t="s">
         <v>123</v>
       </c>
       <c r="H30" s="15"/>
-      <c r="I30" s="31" t="s">
+      <c r="I30" s="26" t="s">
         <v>151</v>
       </c>
-      <c r="J30" s="31" t="s">
-        <v>57</v>
-      </c>
-      <c r="K30" s="31" t="s">
+      <c r="J30" s="26" t="s">
+        <v>57</v>
+      </c>
+      <c r="K30" s="26" t="s">
         <v>167</v>
       </c>
     </row>
@@ -2312,32 +2317,32 @@
         <f>ROW(A31) - ROW($A$10)</f>
         <v>21</v>
       </c>
-      <c r="B31" s="30" t="s">
+      <c r="B31" s="25" t="s">
         <v>34</v>
       </c>
       <c r="C31" s="14">
         <v>2</v>
       </c>
-      <c r="D31" s="30" t="s">
-        <v>57</v>
-      </c>
-      <c r="E31" s="30" t="s">
-        <v>57</v>
-      </c>
-      <c r="F31" s="30" t="s">
+      <c r="D31" s="25" t="s">
+        <v>57</v>
+      </c>
+      <c r="E31" s="25" t="s">
+        <v>57</v>
+      </c>
+      <c r="F31" s="25" t="s">
         <v>83</v>
       </c>
-      <c r="G31" s="31" t="s">
+      <c r="G31" s="26" t="s">
         <v>124</v>
       </c>
       <c r="H31" s="15"/>
-      <c r="I31" s="31" t="s">
+      <c r="I31" s="26" t="s">
         <v>145</v>
       </c>
-      <c r="J31" s="31" t="s">
-        <v>57</v>
-      </c>
-      <c r="K31" s="31" t="s">
+      <c r="J31" s="26" t="s">
+        <v>57</v>
+      </c>
+      <c r="K31" s="26" t="s">
         <v>167</v>
       </c>
     </row>
@@ -2346,32 +2351,32 @@
         <f t="shared" si="0"/>
         <v>22</v>
       </c>
-      <c r="B32" s="30" t="s">
+      <c r="B32" s="25" t="s">
         <v>35</v>
       </c>
       <c r="C32" s="14">
         <v>1</v>
       </c>
-      <c r="D32" s="30" t="s">
-        <v>57</v>
-      </c>
-      <c r="E32" s="30" t="s">
-        <v>57</v>
-      </c>
-      <c r="F32" s="30" t="s">
+      <c r="D32" s="25" t="s">
+        <v>57</v>
+      </c>
+      <c r="E32" s="25" t="s">
+        <v>57</v>
+      </c>
+      <c r="F32" s="25" t="s">
         <v>84</v>
       </c>
-      <c r="G32" s="31" t="s">
+      <c r="G32" s="26" t="s">
         <v>125</v>
       </c>
       <c r="H32" s="15"/>
-      <c r="I32" s="31" t="s">
+      <c r="I32" s="26" t="s">
         <v>152</v>
       </c>
-      <c r="J32" s="31" t="s">
-        <v>57</v>
-      </c>
-      <c r="K32" s="31" t="s">
+      <c r="J32" s="26" t="s">
+        <v>57</v>
+      </c>
+      <c r="K32" s="26" t="s">
         <v>167</v>
       </c>
     </row>
@@ -2380,32 +2385,32 @@
         <f>ROW(A33) - ROW($A$10)</f>
         <v>23</v>
       </c>
-      <c r="B33" s="30" t="s">
+      <c r="B33" s="25" t="s">
         <v>36</v>
       </c>
       <c r="C33" s="14">
         <v>1</v>
       </c>
-      <c r="D33" s="30" t="s">
-        <v>57</v>
-      </c>
-      <c r="E33" s="30" t="s">
-        <v>57</v>
-      </c>
-      <c r="F33" s="30" t="s">
+      <c r="D33" s="25" t="s">
+        <v>57</v>
+      </c>
+      <c r="E33" s="25" t="s">
+        <v>57</v>
+      </c>
+      <c r="F33" s="25" t="s">
         <v>85</v>
       </c>
-      <c r="G33" s="31" t="s">
+      <c r="G33" s="26" t="s">
         <v>126</v>
       </c>
       <c r="H33" s="15"/>
-      <c r="I33" s="31" t="s">
+      <c r="I33" s="26" t="s">
         <v>144</v>
       </c>
-      <c r="J33" s="31" t="s">
-        <v>57</v>
-      </c>
-      <c r="K33" s="31" t="s">
+      <c r="J33" s="26" t="s">
+        <v>57</v>
+      </c>
+      <c r="K33" s="26" t="s">
         <v>167</v>
       </c>
     </row>
@@ -2414,32 +2419,32 @@
         <f t="shared" si="0"/>
         <v>24</v>
       </c>
-      <c r="B34" s="30" t="s">
+      <c r="B34" s="25" t="s">
         <v>37</v>
       </c>
       <c r="C34" s="14">
         <v>1</v>
       </c>
-      <c r="D34" s="30" t="s">
-        <v>57</v>
-      </c>
-      <c r="E34" s="30" t="s">
-        <v>57</v>
-      </c>
-      <c r="F34" s="30" t="s">
+      <c r="D34" s="25" t="s">
+        <v>57</v>
+      </c>
+      <c r="E34" s="25" t="s">
+        <v>57</v>
+      </c>
+      <c r="F34" s="25" t="s">
         <v>86</v>
       </c>
-      <c r="G34" s="31" t="s">
+      <c r="G34" s="26" t="s">
         <v>127</v>
       </c>
       <c r="H34" s="15"/>
-      <c r="I34" s="31" t="s">
+      <c r="I34" s="26" t="s">
         <v>143</v>
       </c>
-      <c r="J34" s="31" t="s">
-        <v>57</v>
-      </c>
-      <c r="K34" s="31" t="s">
+      <c r="J34" s="26" t="s">
+        <v>57</v>
+      </c>
+      <c r="K34" s="26" t="s">
         <v>167</v>
       </c>
     </row>
@@ -2448,32 +2453,32 @@
         <f>ROW(A35) - ROW($A$10)</f>
         <v>25</v>
       </c>
-      <c r="B35" s="30" t="s">
+      <c r="B35" s="25" t="s">
         <v>38</v>
       </c>
       <c r="C35" s="14">
         <v>1</v>
       </c>
-      <c r="D35" s="30" t="s">
-        <v>57</v>
-      </c>
-      <c r="E35" s="30" t="s">
-        <v>57</v>
-      </c>
-      <c r="F35" s="30" t="s">
+      <c r="D35" s="25" t="s">
+        <v>57</v>
+      </c>
+      <c r="E35" s="25" t="s">
+        <v>57</v>
+      </c>
+      <c r="F35" s="25" t="s">
         <v>87</v>
       </c>
-      <c r="G35" s="31" t="s">
+      <c r="G35" s="26" t="s">
         <v>128</v>
       </c>
       <c r="H35" s="15"/>
-      <c r="I35" s="31" t="s">
+      <c r="I35" s="26" t="s">
         <v>144</v>
       </c>
-      <c r="J35" s="31" t="s">
-        <v>57</v>
-      </c>
-      <c r="K35" s="31" t="s">
+      <c r="J35" s="26" t="s">
+        <v>57</v>
+      </c>
+      <c r="K35" s="26" t="s">
         <v>167</v>
       </c>
     </row>
@@ -2482,32 +2487,32 @@
         <f t="shared" si="0"/>
         <v>26</v>
       </c>
-      <c r="B36" s="30" t="s">
+      <c r="B36" s="25" t="s">
         <v>39</v>
       </c>
       <c r="C36" s="14">
         <v>1</v>
       </c>
-      <c r="D36" s="30" t="s">
-        <v>57</v>
-      </c>
-      <c r="E36" s="30" t="s">
-        <v>57</v>
-      </c>
-      <c r="F36" s="30" t="s">
+      <c r="D36" s="25" t="s">
+        <v>57</v>
+      </c>
+      <c r="E36" s="25" t="s">
+        <v>57</v>
+      </c>
+      <c r="F36" s="25" t="s">
         <v>88</v>
       </c>
-      <c r="G36" s="31" t="s">
+      <c r="G36" s="26" t="s">
         <v>129</v>
       </c>
       <c r="H36" s="15"/>
-      <c r="I36" s="31" t="s">
+      <c r="I36" s="26" t="s">
         <v>153</v>
       </c>
-      <c r="J36" s="31" t="s">
-        <v>57</v>
-      </c>
-      <c r="K36" s="31" t="s">
+      <c r="J36" s="26" t="s">
+        <v>57</v>
+      </c>
+      <c r="K36" s="26" t="s">
         <v>167</v>
       </c>
     </row>
@@ -2516,32 +2521,32 @@
         <f>ROW(A37) - ROW($A$10)</f>
         <v>27</v>
       </c>
-      <c r="B37" s="30" t="s">
+      <c r="B37" s="25" t="s">
         <v>40</v>
       </c>
       <c r="C37" s="14">
         <v>1</v>
       </c>
-      <c r="D37" s="30" t="s">
-        <v>57</v>
-      </c>
-      <c r="E37" s="30" t="s">
-        <v>57</v>
-      </c>
-      <c r="F37" s="30" t="s">
+      <c r="D37" s="25" t="s">
+        <v>57</v>
+      </c>
+      <c r="E37" s="25" t="s">
+        <v>57</v>
+      </c>
+      <c r="F37" s="25" t="s">
         <v>89</v>
       </c>
-      <c r="G37" s="31" t="s">
+      <c r="G37" s="26" t="s">
         <v>130</v>
       </c>
       <c r="H37" s="15"/>
-      <c r="I37" s="31" t="s">
+      <c r="I37" s="26" t="s">
         <v>154</v>
       </c>
-      <c r="J37" s="31" t="s">
-        <v>57</v>
-      </c>
-      <c r="K37" s="31" t="s">
+      <c r="J37" s="26" t="s">
+        <v>57</v>
+      </c>
+      <c r="K37" s="26" t="s">
         <v>167</v>
       </c>
     </row>
@@ -2550,32 +2555,32 @@
         <f t="shared" si="0"/>
         <v>28</v>
       </c>
-      <c r="B38" s="30" t="s">
+      <c r="B38" s="25" t="s">
         <v>41</v>
       </c>
       <c r="C38" s="14">
         <v>1</v>
       </c>
-      <c r="D38" s="30" t="s">
-        <v>57</v>
-      </c>
-      <c r="E38" s="30" t="s">
-        <v>57</v>
-      </c>
-      <c r="F38" s="30" t="s">
+      <c r="D38" s="25" t="s">
+        <v>57</v>
+      </c>
+      <c r="E38" s="25" t="s">
+        <v>57</v>
+      </c>
+      <c r="F38" s="25" t="s">
         <v>90</v>
       </c>
-      <c r="G38" s="31" t="s">
+      <c r="G38" s="26" t="s">
         <v>131</v>
       </c>
       <c r="H38" s="15"/>
-      <c r="I38" s="31" t="s">
+      <c r="I38" s="26" t="s">
         <v>143</v>
       </c>
-      <c r="J38" s="31" t="s">
-        <v>57</v>
-      </c>
-      <c r="K38" s="31" t="s">
+      <c r="J38" s="26" t="s">
+        <v>57</v>
+      </c>
+      <c r="K38" s="26" t="s">
         <v>167</v>
       </c>
     </row>
@@ -2584,32 +2589,32 @@
         <f>ROW(A39) - ROW($A$10)</f>
         <v>29</v>
       </c>
-      <c r="B39" s="30" t="s">
+      <c r="B39" s="25" t="s">
         <v>42</v>
       </c>
       <c r="C39" s="14">
         <v>1</v>
       </c>
-      <c r="D39" s="30" t="s">
-        <v>57</v>
-      </c>
-      <c r="E39" s="30" t="s">
-        <v>57</v>
-      </c>
-      <c r="F39" s="30" t="s">
+      <c r="D39" s="25" t="s">
+        <v>57</v>
+      </c>
+      <c r="E39" s="25" t="s">
+        <v>57</v>
+      </c>
+      <c r="F39" s="25" t="s">
         <v>91</v>
       </c>
-      <c r="G39" s="31" t="s">
+      <c r="G39" s="26" t="s">
         <v>132</v>
       </c>
       <c r="H39" s="15"/>
-      <c r="I39" s="31" t="s">
+      <c r="I39" s="26" t="s">
         <v>147</v>
       </c>
-      <c r="J39" s="31" t="s">
-        <v>57</v>
-      </c>
-      <c r="K39" s="31" t="s">
+      <c r="J39" s="26" t="s">
+        <v>57</v>
+      </c>
+      <c r="K39" s="26" t="s">
         <v>167</v>
       </c>
     </row>
@@ -2618,32 +2623,32 @@
         <f t="shared" si="0"/>
         <v>30</v>
       </c>
-      <c r="B40" s="30" t="s">
+      <c r="B40" s="25" t="s">
         <v>43</v>
       </c>
       <c r="C40" s="14">
         <v>1</v>
       </c>
-      <c r="D40" s="30" t="s">
-        <v>57</v>
-      </c>
-      <c r="E40" s="30" t="s">
-        <v>57</v>
-      </c>
-      <c r="F40" s="30" t="s">
+      <c r="D40" s="25" t="s">
+        <v>57</v>
+      </c>
+      <c r="E40" s="25" t="s">
+        <v>57</v>
+      </c>
+      <c r="F40" s="25" t="s">
         <v>92</v>
       </c>
-      <c r="G40" s="31" t="s">
+      <c r="G40" s="26" t="s">
         <v>133</v>
       </c>
       <c r="H40" s="15"/>
-      <c r="I40" s="31" t="s">
+      <c r="I40" s="26" t="s">
         <v>155</v>
       </c>
-      <c r="J40" s="31" t="s">
-        <v>57</v>
-      </c>
-      <c r="K40" s="31" t="s">
+      <c r="J40" s="26" t="s">
+        <v>57</v>
+      </c>
+      <c r="K40" s="26" t="s">
         <v>167</v>
       </c>
     </row>
@@ -2652,32 +2657,32 @@
         <f>ROW(A41) - ROW($A$10)</f>
         <v>31</v>
       </c>
-      <c r="B41" s="30" t="s">
+      <c r="B41" s="25" t="s">
         <v>44</v>
       </c>
       <c r="C41" s="14">
         <v>1</v>
       </c>
-      <c r="D41" s="30" t="s">
+      <c r="D41" s="25" t="s">
         <v>58</v>
       </c>
-      <c r="E41" s="30" t="s">
+      <c r="E41" s="25" t="s">
         <v>61</v>
       </c>
-      <c r="F41" s="30" t="s">
-        <v>57</v>
-      </c>
-      <c r="G41" s="31" t="s">
+      <c r="F41" s="25" t="s">
+        <v>57</v>
+      </c>
+      <c r="G41" s="26" t="s">
         <v>134</v>
       </c>
       <c r="H41" s="15"/>
-      <c r="I41" s="31" t="s">
+      <c r="I41" s="26" t="s">
         <v>156</v>
       </c>
-      <c r="J41" s="31" t="s">
+      <c r="J41" s="26" t="s">
         <v>166</v>
       </c>
-      <c r="K41" s="31" t="s">
+      <c r="K41" s="26" t="s">
         <v>167</v>
       </c>
     </row>
@@ -2686,32 +2691,32 @@
         <f t="shared" si="0"/>
         <v>32</v>
       </c>
-      <c r="B42" s="30" t="s">
+      <c r="B42" s="25" t="s">
         <v>45</v>
       </c>
       <c r="C42" s="14">
         <v>1</v>
       </c>
-      <c r="D42" s="30" t="s">
-        <v>57</v>
-      </c>
-      <c r="E42" s="30" t="s">
-        <v>57</v>
-      </c>
-      <c r="F42" s="30" t="s">
+      <c r="D42" s="25" t="s">
+        <v>57</v>
+      </c>
+      <c r="E42" s="25" t="s">
+        <v>57</v>
+      </c>
+      <c r="F42" s="25" t="s">
         <v>93</v>
       </c>
-      <c r="G42" s="31" t="s">
+      <c r="G42" s="26" t="s">
         <v>135</v>
       </c>
       <c r="H42" s="15"/>
-      <c r="I42" s="31" t="s">
+      <c r="I42" s="26" t="s">
         <v>157</v>
       </c>
-      <c r="J42" s="31" t="s">
-        <v>57</v>
-      </c>
-      <c r="K42" s="31" t="s">
+      <c r="J42" s="26" t="s">
+        <v>57</v>
+      </c>
+      <c r="K42" s="26" t="s">
         <v>167</v>
       </c>
     </row>
@@ -2720,32 +2725,32 @@
         <f>ROW(A43) - ROW($A$10)</f>
         <v>33</v>
       </c>
-      <c r="B43" s="30" t="s">
+      <c r="B43" s="25" t="s">
         <v>46</v>
       </c>
       <c r="C43" s="14">
         <v>1</v>
       </c>
-      <c r="D43" s="30" t="s">
-        <v>57</v>
-      </c>
-      <c r="E43" s="30" t="s">
-        <v>57</v>
-      </c>
-      <c r="F43" s="30" t="s">
+      <c r="D43" s="25" t="s">
+        <v>57</v>
+      </c>
+      <c r="E43" s="25" t="s">
+        <v>57</v>
+      </c>
+      <c r="F43" s="25" t="s">
         <v>94</v>
       </c>
-      <c r="G43" s="31" t="s">
+      <c r="G43" s="26" t="s">
         <v>136</v>
       </c>
       <c r="H43" s="15"/>
-      <c r="I43" s="31" t="s">
+      <c r="I43" s="26" t="s">
         <v>158</v>
       </c>
-      <c r="J43" s="31" t="s">
-        <v>57</v>
-      </c>
-      <c r="K43" s="31" t="s">
+      <c r="J43" s="26" t="s">
+        <v>57</v>
+      </c>
+      <c r="K43" s="26" t="s">
         <v>167</v>
       </c>
     </row>
@@ -2754,32 +2759,32 @@
         <f t="shared" si="0"/>
         <v>34</v>
       </c>
-      <c r="B44" s="30" t="s">
+      <c r="B44" s="25" t="s">
         <v>47</v>
       </c>
       <c r="C44" s="14">
         <v>1</v>
       </c>
-      <c r="D44" s="30" t="s">
-        <v>57</v>
-      </c>
-      <c r="E44" s="30" t="s">
-        <v>57</v>
-      </c>
-      <c r="F44" s="30" t="s">
+      <c r="D44" s="25" t="s">
+        <v>57</v>
+      </c>
+      <c r="E44" s="25" t="s">
+        <v>57</v>
+      </c>
+      <c r="F44" s="25" t="s">
         <v>95</v>
       </c>
-      <c r="G44" s="31" t="s">
+      <c r="G44" s="26" t="s">
         <v>95</v>
       </c>
       <c r="H44" s="15"/>
-      <c r="I44" s="31" t="s">
+      <c r="I44" s="26" t="s">
         <v>159</v>
       </c>
-      <c r="J44" s="31" t="s">
-        <v>57</v>
-      </c>
-      <c r="K44" s="31" t="s">
+      <c r="J44" s="26" t="s">
+        <v>57</v>
+      </c>
+      <c r="K44" s="26" t="s">
         <v>167</v>
       </c>
     </row>
@@ -2788,32 +2793,32 @@
         <f>ROW(A45) - ROW($A$10)</f>
         <v>35</v>
       </c>
-      <c r="B45" s="30" t="s">
+      <c r="B45" s="25" t="s">
         <v>48</v>
       </c>
       <c r="C45" s="14">
         <v>1</v>
       </c>
-      <c r="D45" s="30" t="s">
+      <c r="D45" s="25" t="s">
         <v>59</v>
       </c>
-      <c r="E45" s="30" t="s">
-        <v>57</v>
-      </c>
-      <c r="F45" s="30" t="s">
+      <c r="E45" s="25" t="s">
+        <v>57</v>
+      </c>
+      <c r="F45" s="25" t="s">
         <v>96</v>
       </c>
-      <c r="G45" s="31" t="s">
+      <c r="G45" s="26" t="s">
         <v>137</v>
       </c>
       <c r="H45" s="15"/>
-      <c r="I45" s="31" t="s">
+      <c r="I45" s="26" t="s">
         <v>160</v>
       </c>
-      <c r="J45" s="31" t="s">
-        <v>57</v>
-      </c>
-      <c r="K45" s="31" t="s">
+      <c r="J45" s="26" t="s">
+        <v>57</v>
+      </c>
+      <c r="K45" s="26" t="s">
         <v>167</v>
       </c>
     </row>
@@ -2822,32 +2827,32 @@
         <f t="shared" si="0"/>
         <v>36</v>
       </c>
-      <c r="B46" s="30" t="s">
+      <c r="B46" s="25" t="s">
         <v>49</v>
       </c>
       <c r="C46" s="14">
         <v>1</v>
       </c>
-      <c r="D46" s="30" t="s">
-        <v>57</v>
-      </c>
-      <c r="E46" s="30" t="s">
-        <v>57</v>
-      </c>
-      <c r="F46" s="30" t="s">
+      <c r="D46" s="25" t="s">
+        <v>57</v>
+      </c>
+      <c r="E46" s="25" t="s">
+        <v>57</v>
+      </c>
+      <c r="F46" s="25" t="s">
         <v>97</v>
       </c>
-      <c r="G46" s="31" t="s">
+      <c r="G46" s="26" t="s">
         <v>138</v>
       </c>
       <c r="H46" s="15"/>
-      <c r="I46" s="31" t="s">
+      <c r="I46" s="26" t="s">
         <v>161</v>
       </c>
-      <c r="J46" s="31" t="s">
-        <v>57</v>
-      </c>
-      <c r="K46" s="31" t="s">
+      <c r="J46" s="26" t="s">
+        <v>57</v>
+      </c>
+      <c r="K46" s="26" t="s">
         <v>167</v>
       </c>
     </row>
@@ -2856,32 +2861,32 @@
         <f>ROW(A47) - ROW($A$10)</f>
         <v>37</v>
       </c>
-      <c r="B47" s="30" t="s">
+      <c r="B47" s="25" t="s">
         <v>50</v>
       </c>
       <c r="C47" s="14">
         <v>1</v>
       </c>
-      <c r="D47" s="30" t="s">
-        <v>57</v>
-      </c>
-      <c r="E47" s="30" t="s">
-        <v>57</v>
-      </c>
-      <c r="F47" s="30" t="s">
+      <c r="D47" s="25" t="s">
+        <v>57</v>
+      </c>
+      <c r="E47" s="25" t="s">
+        <v>57</v>
+      </c>
+      <c r="F47" s="25" t="s">
         <v>98</v>
       </c>
-      <c r="G47" s="31" t="s">
+      <c r="G47" s="26" t="s">
         <v>98</v>
       </c>
       <c r="H47" s="15"/>
-      <c r="I47" s="31" t="s">
+      <c r="I47" s="26" t="s">
         <v>162</v>
       </c>
-      <c r="J47" s="31" t="s">
-        <v>57</v>
-      </c>
-      <c r="K47" s="31" t="s">
+      <c r="J47" s="26" t="s">
+        <v>57</v>
+      </c>
+      <c r="K47" s="26" t="s">
         <v>167</v>
       </c>
     </row>
@@ -2890,32 +2895,32 @@
         <f t="shared" si="0"/>
         <v>38</v>
       </c>
-      <c r="B48" s="30" t="s">
+      <c r="B48" s="25" t="s">
         <v>51</v>
       </c>
       <c r="C48" s="14">
-        <v>1</v>
-      </c>
-      <c r="D48" s="30" t="s">
-        <v>57</v>
-      </c>
-      <c r="E48" s="30" t="s">
-        <v>57</v>
-      </c>
-      <c r="F48" s="30" t="s">
+        <v>2</v>
+      </c>
+      <c r="D48" s="25" t="s">
+        <v>57</v>
+      </c>
+      <c r="E48" s="25" t="s">
+        <v>57</v>
+      </c>
+      <c r="F48" s="25" t="s">
         <v>99</v>
       </c>
-      <c r="G48" s="31" t="s">
+      <c r="G48" s="26" t="s">
         <v>51</v>
       </c>
       <c r="H48" s="15"/>
-      <c r="I48" s="31" t="s">
+      <c r="I48" s="26" t="s">
         <v>51</v>
       </c>
-      <c r="J48" s="31" t="s">
-        <v>57</v>
-      </c>
-      <c r="K48" s="31" t="s">
+      <c r="J48" s="26" t="s">
+        <v>57</v>
+      </c>
+      <c r="K48" s="26" t="s">
         <v>167</v>
       </c>
     </row>
@@ -2924,32 +2929,32 @@
         <f>ROW(A49) - ROW($A$10)</f>
         <v>39</v>
       </c>
-      <c r="B49" s="30" t="s">
+      <c r="B49" s="25" t="s">
         <v>52</v>
       </c>
       <c r="C49" s="14">
         <v>1</v>
       </c>
-      <c r="D49" s="30" t="s">
-        <v>57</v>
-      </c>
-      <c r="E49" s="30" t="s">
-        <v>57</v>
-      </c>
-      <c r="F49" s="30" t="s">
+      <c r="D49" s="25" t="s">
+        <v>57</v>
+      </c>
+      <c r="E49" s="25" t="s">
+        <v>57</v>
+      </c>
+      <c r="F49" s="25" t="s">
         <v>100</v>
       </c>
-      <c r="G49" s="31" t="s">
+      <c r="G49" s="26" t="s">
         <v>139</v>
       </c>
       <c r="H49" s="15"/>
-      <c r="I49" s="31" t="s">
+      <c r="I49" s="26" t="s">
         <v>147</v>
       </c>
-      <c r="J49" s="31" t="s">
-        <v>57</v>
-      </c>
-      <c r="K49" s="31" t="s">
+      <c r="J49" s="26" t="s">
+        <v>57</v>
+      </c>
+      <c r="K49" s="26" t="s">
         <v>167</v>
       </c>
     </row>
@@ -2958,32 +2963,32 @@
         <f t="shared" si="0"/>
         <v>40</v>
       </c>
-      <c r="B50" s="30" t="s">
+      <c r="B50" s="25" t="s">
         <v>53</v>
       </c>
       <c r="C50" s="14">
         <v>1</v>
       </c>
-      <c r="D50" s="30" t="s">
-        <v>57</v>
-      </c>
-      <c r="E50" s="30" t="s">
-        <v>57</v>
-      </c>
-      <c r="F50" s="30" t="s">
+      <c r="D50" s="25" t="s">
+        <v>57</v>
+      </c>
+      <c r="E50" s="25" t="s">
+        <v>57</v>
+      </c>
+      <c r="F50" s="25" t="s">
         <v>101</v>
       </c>
-      <c r="G50" s="31" t="s">
+      <c r="G50" s="26" t="s">
         <v>101</v>
       </c>
       <c r="H50" s="15"/>
-      <c r="I50" s="31" t="s">
+      <c r="I50" s="26" t="s">
         <v>163</v>
       </c>
-      <c r="J50" s="31" t="s">
-        <v>57</v>
-      </c>
-      <c r="K50" s="31" t="s">
+      <c r="J50" s="26" t="s">
+        <v>57</v>
+      </c>
+      <c r="K50" s="26" t="s">
         <v>167</v>
       </c>
     </row>
@@ -2992,32 +2997,32 @@
         <f>ROW(A51) - ROW($A$10)</f>
         <v>41</v>
       </c>
-      <c r="B51" s="30" t="s">
+      <c r="B51" s="25" t="s">
         <v>54</v>
       </c>
       <c r="C51" s="14">
         <v>1</v>
       </c>
-      <c r="D51" s="30" t="s">
+      <c r="D51" s="25" t="s">
         <v>59</v>
       </c>
-      <c r="E51" s="30" t="s">
-        <v>57</v>
-      </c>
-      <c r="F51" s="30" t="s">
+      <c r="E51" s="25" t="s">
+        <v>57</v>
+      </c>
+      <c r="F51" s="25" t="s">
         <v>102</v>
       </c>
-      <c r="G51" s="31" t="s">
+      <c r="G51" s="26" t="s">
         <v>140</v>
       </c>
       <c r="H51" s="15"/>
-      <c r="I51" s="31" t="s">
+      <c r="I51" s="26" t="s">
         <v>164</v>
       </c>
-      <c r="J51" s="31" t="s">
-        <v>57</v>
-      </c>
-      <c r="K51" s="31" t="s">
+      <c r="J51" s="26" t="s">
+        <v>57</v>
+      </c>
+      <c r="K51" s="26" t="s">
         <v>167</v>
       </c>
     </row>

</xml_diff>